<commit_message>
Added data audit and data catalog to gea.py
</commit_message>
<xml_diff>
--- a/model_config.xlsx
+++ b/model_config.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asafsilman/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asafsilman/Desktop/GENG5511/GalaxyEnvironmentAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754451DD-13A1-7F4C-843A-4A58DEAF5FDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1768811B-DBE9-4B45-BD97-31533BE08F9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-11880" windowWidth="38400" windowHeight="21140" xr2:uid="{DA573336-42C9-534D-A3C9-C8C047CC3E2B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" activeTab="1" xr2:uid="{DA573336-42C9-534D-A3C9-C8C047CC3E2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="1" r:id="rId1"/>
-    <sheet name="DataSources" sheetId="2" r:id="rId2"/>
+    <sheet name="DataFiles" sheetId="2" r:id="rId2"/>
     <sheet name="DataLabels" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="181">
   <si>
     <t>modelName</t>
   </si>
@@ -374,13 +374,217 @@
   </si>
   <si>
     <t>dataSetLabel</t>
+  </si>
+  <si>
+    <t>025612e8900f463e844175fa92bd17ce091bf685f3703693e7131ff205c09505</t>
+  </si>
+  <si>
+    <t>71562c1f35024ebcabc103b3a63902ef6995fc2c49656746ab6973912a3d403e</t>
+  </si>
+  <si>
+    <t>67c90ef5e134bfbc35babacfe6b7bcb293bfc9d1cef05aa4f4626f4bbf602279</t>
+  </si>
+  <si>
+    <t>8289cdbdc884f8499f1e5f5354fd653ab3e19f1c6a8d7d9c1bd099339ae97d33</t>
+  </si>
+  <si>
+    <t>887de8292fde032606cbeb45b3afa3e0a36cc2ddbeb073f8f697f5b54442c307</t>
+  </si>
+  <si>
+    <t>e6dfc0ebc2c5c2f68cfc0379e0abb2435a6a6c50f20aab32c9b286d3f17a2d72</t>
+  </si>
+  <si>
+    <t>9b384fe0e289cfadb9d489ef2d5baaffa520c70d748b480aeb4ece9714e7fcbb</t>
+  </si>
+  <si>
+    <t>5c679999b14b678db312752564543ba05c47b970b6aa1c846f4daf9d7a53f242</t>
+  </si>
+  <si>
+    <t>9c250155539c47a02e9d5bcba736f21921d4b8d8f1a19cd3fcbc2d5232012200</t>
+  </si>
+  <si>
+    <t>c797b27d0cbd370a4734c7a0a649394024445f39a92903970d7a0f5e36eb6516</t>
+  </si>
+  <si>
+    <t>5c708abe468e04542b3f513f8f9fadf31d85b4f6dbf32985db5fd7fa6aaaad50</t>
+  </si>
+  <si>
+    <t>45862088c1a6dc79ba30555563eb9599381f99cc6e9545f0c033c40f5e23e8b7</t>
+  </si>
+  <si>
+    <t>b7d9aadfae4ace0ec88bf1b4251b8734baff158f55577a4625cb94ddca42ac87</t>
+  </si>
+  <si>
+    <t>fd9cb90c358fcaeb5498935fdbb54b21e41caad13fd13618d2a85a3469b3a094</t>
+  </si>
+  <si>
+    <t>ebb97ce1a03331fa4a296b1cc1bb73f1ed88be0541686d2af5ff9770cace317d</t>
+  </si>
+  <si>
+    <t>48d800a1000040dd0508f3147b2f73439d5acde3885f3244c01123dfcb82b786</t>
+  </si>
+  <si>
+    <t>d3a60dcd97b94d3d151a88db3d26a9e8b830ff7518f9fd746502da16e10f4e97</t>
+  </si>
+  <si>
+    <t>da71763701e4dc5b9e9005e2ae8d5036f72d253a8cc83baa79ce2094913e7f90</t>
+  </si>
+  <si>
+    <t>004ad7e51823f4b11c2bed0a49b1710c34e6a4720e4061fca5d1f48703c37153</t>
+  </si>
+  <si>
+    <t>9e0bde26c1ca7fe3199c4bcce2c533d44077703acf53bd6bd7855fa6ecf40a3e</t>
+  </si>
+  <si>
+    <t>c4dfcc64b5557fabb90a0a817ba9608e03e3f8427262e57435cf9446593a76e9</t>
+  </si>
+  <si>
+    <t>ca17d90d9f123258a3e2f14ab5c11f8533a4bad6013500386406e0efe1d6b06a</t>
+  </si>
+  <si>
+    <t>189a84a4fd1520f2575e6a51063013b08bda7ab39cdb5d1fe06105ee3f5b1be7</t>
+  </si>
+  <si>
+    <t>3d94e7891182502c38eacd4202df33886484193657957567b3b64705ce88a609</t>
+  </si>
+  <si>
+    <t>a5af1dda0ed219303b53f1b60b435b6f1861a99fe9083be9523a574085db23a1</t>
+  </si>
+  <si>
+    <t>2e228cf630ede1f501cf48f086d3b637bcbb1638ac38cfd926fef55d89e398d2</t>
+  </si>
+  <si>
+    <t>d3067e32851de9d5086d1fb0ca4eded1863ddd3437dcdb4d093ea17b3baed46b</t>
+  </si>
+  <si>
+    <t>8821643151e5110c7e240a7ae2c45738b52258ae4b6bbe0da747fd0aeb11903c</t>
+  </si>
+  <si>
+    <t>94e1734d527da61d24d5ae0da6f0d1bdb0e5b0d2ab64db748d74502b7b957057</t>
+  </si>
+  <si>
+    <t>3244fa021f83328102ccc78394235449d25957e3548a83fc2a13475bd26f798d</t>
+  </si>
+  <si>
+    <t>8de36be9b3818d4f4b28c82ba4d7442463ee931d9877ac3f4c217987c7625902</t>
+  </si>
+  <si>
+    <t>b643daf18ba8f463150db841aaf3b6ce720033c87655f157b9180e672af9e3f0</t>
+  </si>
+  <si>
+    <t>f87bcb055e1d074393b7c94eaa4eee57de0b110c45b1c686c8337eea124fc297</t>
+  </si>
+  <si>
+    <t>8999a7e050c00c187fb7c4abaab86cdc51ed60d61aee6571fcb1946dc391c163</t>
+  </si>
+  <si>
+    <t>6657d951329c6df4402ab1f301f13dcd11b3b53eee6186c740746b4342e44f6f</t>
+  </si>
+  <si>
+    <t>1c3b3408a3da35891fa3714225e416458ffa1f277724a07be8ccc3d69c506e5e</t>
+  </si>
+  <si>
+    <t>d40fb0e22bd8dd1ec1974218c69103f0c7deb53079f68d01cf102b482a7f828f</t>
+  </si>
+  <si>
+    <t>35aea4b5103e7e9fdd94ff78f9b0fe46931eeedcacfc720a8e58952fd549d00c</t>
+  </si>
+  <si>
+    <t>54f34161e3695b6f566c51e7d7941450c5ce43e02f0983cec83417380422e786</t>
+  </si>
+  <si>
+    <t>e1b42fe76c08c168e1756b44d73f77f94ae48b3ff9c481a050bcf082963c4cdb</t>
+  </si>
+  <si>
+    <t>9f1310785acfbd8ea148eefa208f1a546ca9a7ec362c121ff585fd64dff79599</t>
+  </si>
+  <si>
+    <t>77299bec6599a5fe00be7df2b1a26bb30808827d04134fff3302bd7b37bebd18</t>
+  </si>
+  <si>
+    <t>m1v.dir/2dft.dat</t>
+  </si>
+  <si>
+    <t>m1v.dir/2dftn1.dat</t>
+  </si>
+  <si>
+    <t>4d5839c3e39cdb8a126b63eb3db98966f39fac2805bb8b1e087dbd5f3da691ee</t>
+  </si>
+  <si>
+    <t>7421eea217b08ffd50031680bd87460b5c8ef499ed135b638a522a81aaa9c303</t>
+  </si>
+  <si>
+    <t>1a35dda72518633543e90d48a9ab797125a6041b3f3e2ba8cae370def93e5a01</t>
+  </si>
+  <si>
+    <t>ae2bbaa6164149ebda3d39b508d49c21c4f1ef44ddfdae92346c8c7d311bf385</t>
+  </si>
+  <si>
+    <t>3c9bc5fa4985eb6eacc9013a7df9cb7c99bdf072b37040166da7488d8e97de28</t>
+  </si>
+  <si>
+    <t>359b195613f8432e4a302444e12fdb99b4aab5412910bc2cb6a5c842f6636b77</t>
+  </si>
+  <si>
+    <t>95a5121eb3258849b8d01aa9f7cb790580d79fc80954654fe00a8ec7b60479d7</t>
+  </si>
+  <si>
+    <t>eb3d056f54c2eaefb103b6ab84950ffeed0ee19a536ad3b314d541c6ba339052</t>
+  </si>
+  <si>
+    <t>ac8bc3cee962b96a0ae5ea3473ff5d79884ecd4e011cfdc26db8c5ff3c4cd5ff</t>
+  </si>
+  <si>
+    <t>664aa26039891520cc86511a6777429d42eab7d2d8cbc1d3be3863c58f9435d8</t>
+  </si>
+  <si>
+    <t>468f29693595758ad6df2be69aef023af8fb5ce9eb3f6fa8ebfd54015b91b10e</t>
+  </si>
+  <si>
+    <t>05a16a3faf932960d584a5d7946b7932508df5a57f3b7f14f554b06051c3b14a</t>
+  </si>
+  <si>
+    <t>7da6e04f5374d0e8d616ce4845600700d5f7d098f4738f977e8b4e44de0ab6fb</t>
+  </si>
+  <si>
+    <t>b1af1a311d271d88bb01c5f64d4b40a1b9b679f799a1a0c347858ad0cab6079c</t>
+  </si>
+  <si>
+    <t>8b75d36fec2fcd89269e5121420def87965bca9519a77b5c357e20e2fba79581</t>
+  </si>
+  <si>
+    <t>90ffc2205ea8f06d4f1e59a83d43659c4b12deb010a3dcc3883a1ed8abbd03b3</t>
+  </si>
+  <si>
+    <t>8395d5840feb547b42c6fc7c5cd6e5bf1d6f6acf07a7d43aeca1acb316e6f40f</t>
+  </si>
+  <si>
+    <t>ff3c50d8c174f4eed2bc2ec5e89065154b55a2a516dc83f0cea5ceee51c28cd9</t>
+  </si>
+  <si>
+    <t>5742f81b7e2fe9a5d74193c0346029ed42083a8a65543f58d845c27182c9883e</t>
+  </si>
+  <si>
+    <t>affd0d37f6ae919733bd85908a7276f26307820c1584bd9665c4d6479e3359d5</t>
+  </si>
+  <si>
+    <t>2c5d5e377f37e03b5557d46e0e674def199bef152812147df6dfbe4145e94b5d</t>
+  </si>
+  <si>
+    <t>5bfb3061e68dc5cd27612d3dfc0e41ccfebdb9b965c435c046b4f2b4a1b6cd22</t>
+  </si>
+  <si>
+    <t>d51bddf3784ae121842c96c3329f8aea8f72e7456074e275153a43199efb87df</t>
+  </si>
+  <si>
+    <t>82c6cc0cf6f8a9362eb48ebd3605db263c32a8ac9267b3931a7cf853e2f4c114</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -393,6 +597,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -415,7 +625,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -428,26 +638,46 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -476,6 +706,16 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -495,21 +735,21 @@
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{703C2328-6727-224A-92DA-FB21A475BF4C}" name="modelId"/>
     <tableColumn id="5" xr3:uid="{091AFF89-BAE7-674D-85D8-5FA5B7DAF36C}" name="modelAltName"/>
-    <tableColumn id="6" xr3:uid="{9243668A-FEFC-2A44-85FD-E9850DCD3F13}" name="modelName" dataDxfId="11">
+    <tableColumn id="6" xr3:uid="{9243668A-FEFC-2A44-85FD-E9850DCD3F13}" name="modelName" dataDxfId="12">
       <calculatedColumnFormula>_xlfn.CONCAT(Table3[[#This Row],[numChannels]],"_channel_",Table3[[#This Row],[modelType]],"_", Table3[[#This Row],[_modelNameString]], "_", Table3[[#This Row],[_modelDataString]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{E6DF2D56-96C3-AF43-9D19-75691A5B5160}" name="_modelNameString" dataDxfId="10">
+    <tableColumn id="20" xr3:uid="{E6DF2D56-96C3-AF43-9D19-75691A5B5160}" name="_modelNameString" dataDxfId="11">
       <calculatedColumnFormula>_xlfn.CONCAT(Table3[[#This Row],[channel_1]], IF(Table3[[#This Row],[channel_2]]&lt;&gt;"", _xlfn.CONCAT("_",Table3[[#This Row],[channel_2]], IF(Table3[[#This Row],[channel_3]]&lt;&gt;"", _xlfn.CONCAT("_", Table3[[#This Row],[channel_3]]), ""), ""), ""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{25197AF6-7EB6-9344-B947-E907FA36108D}" name="_modelDataString" dataDxfId="9">
+    <tableColumn id="21" xr3:uid="{25197AF6-7EB6-9344-B947-E907FA36108D}" name="_modelDataString" dataDxfId="10">
       <calculatedColumnFormula>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{A721B211-0E17-F640-A300-BE3E08E93596}" name="modelType" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{4347DEF6-17C0-3F43-802E-86E8674A6FB3}" name="numChannels" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{3B4B9348-11DD-394A-9D6A-D4850CC40194}" name="channel_1" dataDxfId="6"/>
-    <tableColumn id="14" xr3:uid="{B526A24F-2ECC-0442-9CEB-DA811FF165E2}" name="channel_2" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{0052B57A-E822-0B40-8C1E-8D026B8A57CC}" name="channel_3" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{7E2B00ED-F5EB-4648-9E53-8AB3EC8A396B}" name="channel_4" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{A721B211-0E17-F640-A300-BE3E08E93596}" name="modelType" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{4347DEF6-17C0-3F43-802E-86E8674A6FB3}" name="numChannels" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{3B4B9348-11DD-394A-9D6A-D4850CC40194}" name="channel_1" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{B526A24F-2ECC-0442-9CEB-DA811FF165E2}" name="channel_2" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{0052B57A-E822-0B40-8C1E-8D026B8A57CC}" name="channel_3" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{7E2B00ED-F5EB-4648-9E53-8AB3EC8A396B}" name="channel_4" dataDxfId="4"/>
     <tableColumn id="9" xr3:uid="{712BD42A-DEBB-2545-A3FE-8F98C541BB5F}" name="dataSet_m1"/>
     <tableColumn id="10" xr3:uid="{1C7EA2DE-42E0-4949-B9B8-64BD2A71AC95}" name="dataSet_m2"/>
     <tableColumn id="11" xr3:uid="{82D55CF4-DECF-6844-ABEC-7EC6D1BC5DA6}" name="dataSet_m3"/>
@@ -522,11 +762,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BBA15079-BA5C-4347-AB18-D63DE85A40E7}" name="Table1" displayName="Table1" ref="A1:L73" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BBA15079-BA5C-4347-AB18-D63DE85A40E7}" name="Table1" displayName="Table1" ref="A1:L73" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:L73" xr:uid="{1608FF67-3914-5949-96DC-606C50EA2E4D}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{AE589D12-F9F2-7E46-B3F1-011FE87BB9E7}" name="dataId"/>
-    <tableColumn id="2" xr3:uid="{86A820C4-44CA-F647-A338-3C42F8D54CAF}" name="dataFile"/>
+    <tableColumn id="2" xr3:uid="{86A820C4-44CA-F647-A338-3C42F8D54CAF}" name="dataFile" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{8CB7439C-328A-4840-8650-53C68739CB52}" name="dataLabel"/>
     <tableColumn id="6" xr3:uid="{20416ED2-C6CE-DB4D-BCD0-4920296FFAB5}" name="dataLabelValue" dataDxfId="2">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</calculatedColumnFormula>
@@ -536,7 +776,7 @@
     <tableColumn id="7" xr3:uid="{A34CD7B0-6947-5A42-AD6C-DDCF954D6599}" name="imageFileName"/>
     <tableColumn id="8" xr3:uid="{4E77CFD9-0959-1946-94BB-C03C9823FFCF}" name="labelFileName"/>
     <tableColumn id="10" xr3:uid="{B5582984-20BB-B04C-ACD1-B32B5C014342}" name="fileAvailable"/>
-    <tableColumn id="9" xr3:uid="{8E67EC6E-99AC-7043-8F51-B1C73A2D564B}" name="fileHash"/>
+    <tableColumn id="9" xr3:uid="{8E67EC6E-99AC-7043-8F51-B1C73A2D564B}" name="fileHash" dataDxfId="1"/>
     <tableColumn id="11" xr3:uid="{38F53538-5DB0-E34C-B916-D0BD7FD2CC71}" name="imageFileNumRows"/>
     <tableColumn id="12" xr3:uid="{E263E244-E409-B344-BD21-61A040BA1A1C}" name="labelFileNumRows"/>
   </tableColumns>
@@ -854,8 +1094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F969F3E7-5EBB-B140-87B5-F57642023AAB}">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2412,7 +2652,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="L2:Q31">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2427,20 +2667,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A15A60-C633-ED48-8690-686D42EE8C24}">
   <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="G48" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B69" sqref="A69:B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" customWidth="1"/>
-    <col min="7" max="7" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="77.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2487,7 +2726,7 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C2" t="s">
@@ -2509,12 +2748,24 @@
       <c r="H2" t="s">
         <v>39</v>
       </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="K2">
+        <v>1000</v>
+      </c>
+      <c r="L2">
+        <v>1000</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C3" t="s">
@@ -2536,12 +2787,24 @@
       <c r="H3" t="s">
         <v>39</v>
       </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="K3">
+        <v>1000</v>
+      </c>
+      <c r="L3">
+        <v>1000</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C4" t="s">
@@ -2562,13 +2825,25 @@
       </c>
       <c r="H4" t="s">
         <v>39</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="K4">
+        <v>1000</v>
+      </c>
+      <c r="L4">
+        <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="7" t="s">
         <v>44</v>
       </c>
       <c r="C5" t="s">
@@ -2589,13 +2864,25 @@
       </c>
       <c r="H5" t="s">
         <v>39</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="K5">
+        <v>1000</v>
+      </c>
+      <c r="L5">
+        <v>1000</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="7" t="s">
         <v>45</v>
       </c>
       <c r="C6" t="s">
@@ -2616,13 +2903,25 @@
       </c>
       <c r="H6" t="s">
         <v>39</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="K6">
+        <v>1000</v>
+      </c>
+      <c r="L6">
+        <v>1000</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="7" t="s">
         <v>46</v>
       </c>
       <c r="C7" t="s">
@@ -2643,13 +2942,25 @@
       </c>
       <c r="H7" t="s">
         <v>39</v>
+      </c>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="K7">
+        <v>1000</v>
+      </c>
+      <c r="L7">
+        <v>1000</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="7" t="s">
         <v>47</v>
       </c>
       <c r="C8" t="s">
@@ -2670,13 +2981,25 @@
       </c>
       <c r="H8" t="s">
         <v>39</v>
+      </c>
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="K8">
+        <v>1000</v>
+      </c>
+      <c r="L8">
+        <v>1000</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="7" t="s">
         <v>48</v>
       </c>
       <c r="C9" t="s">
@@ -2697,13 +3020,25 @@
       </c>
       <c r="H9" t="s">
         <v>39</v>
+      </c>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="K9">
+        <v>1000</v>
+      </c>
+      <c r="L9">
+        <v>1000</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C10" t="s">
@@ -2724,13 +3059,25 @@
       </c>
       <c r="H10" t="s">
         <v>39</v>
+      </c>
+      <c r="I10" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="K10">
+        <v>1000</v>
+      </c>
+      <c r="L10">
+        <v>1000</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="7" t="s">
         <v>53</v>
       </c>
       <c r="C11" t="s">
@@ -2751,13 +3098,25 @@
       </c>
       <c r="H11" t="s">
         <v>39</v>
+      </c>
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="K11">
+        <v>1000</v>
+      </c>
+      <c r="L11">
+        <v>1000</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C12" t="s">
@@ -2778,13 +3137,25 @@
       </c>
       <c r="H12" t="s">
         <v>39</v>
+      </c>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="K12">
+        <v>1000</v>
+      </c>
+      <c r="L12">
+        <v>1000</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C13" t="s">
@@ -2805,13 +3176,25 @@
       </c>
       <c r="H13" t="s">
         <v>39</v>
+      </c>
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="K13">
+        <v>1000</v>
+      </c>
+      <c r="L13">
+        <v>1000</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C14" t="s">
@@ -2832,13 +3215,25 @@
       </c>
       <c r="H14" t="s">
         <v>39</v>
+      </c>
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="K14">
+        <v>1000</v>
+      </c>
+      <c r="L14">
+        <v>1000</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="7" t="s">
         <v>58</v>
       </c>
       <c r="C15" t="s">
@@ -2855,17 +3250,29 @@
         <v>4</v>
       </c>
       <c r="G15" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="H15" t="s">
-        <v>39</v>
+        <v>156</v>
+      </c>
+      <c r="I15" t="b">
+        <v>1</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="K15">
+        <v>1000</v>
+      </c>
+      <c r="L15">
+        <v>1000</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="7" t="s">
         <v>54</v>
       </c>
       <c r="C16" t="s">
@@ -2887,12 +3294,24 @@
       <c r="H16" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="K16">
+        <v>1000</v>
+      </c>
+      <c r="L16">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="7" t="s">
         <v>59</v>
       </c>
       <c r="C17" t="s">
@@ -2909,17 +3328,29 @@
         <v>4</v>
       </c>
       <c r="G17" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="H17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="I17" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="K17">
+        <v>1000</v>
+      </c>
+      <c r="L17">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="7" t="s">
         <v>60</v>
       </c>
       <c r="C18" t="s">
@@ -2941,12 +3372,24 @@
       <c r="H18" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="K18">
+        <v>1000</v>
+      </c>
+      <c r="L18">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="7" t="s">
         <v>61</v>
       </c>
       <c r="C19" t="s">
@@ -2963,17 +3406,29 @@
         <v>5</v>
       </c>
       <c r="G19" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="H19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="K19">
+        <v>1000</v>
+      </c>
+      <c r="L19">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="7" t="s">
         <v>62</v>
       </c>
       <c r="C20" t="s">
@@ -2995,12 +3450,24 @@
       <c r="H20" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="K20">
+        <v>1000</v>
+      </c>
+      <c r="L20">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="7" t="s">
         <v>63</v>
       </c>
       <c r="C21" t="s">
@@ -3017,17 +3484,29 @@
         <v>5</v>
       </c>
       <c r="G21" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="H21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="I21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="K21">
+        <v>1000</v>
+      </c>
+      <c r="L21">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C22" t="s">
@@ -3049,12 +3528,24 @@
       <c r="H22" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="K22">
+        <v>1000</v>
+      </c>
+      <c r="L22">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C23" t="s">
@@ -3076,12 +3567,24 @@
       <c r="H23" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="K23">
+        <v>1000</v>
+      </c>
+      <c r="L23">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C24" t="s">
@@ -3103,12 +3606,24 @@
       <c r="H24" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="K24">
+        <v>1000</v>
+      </c>
+      <c r="L24">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="7" t="s">
         <v>66</v>
       </c>
       <c r="C25" t="s">
@@ -3125,17 +3640,29 @@
         <v>6</v>
       </c>
       <c r="G25" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="H25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="I25" t="b">
+        <v>1</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="K25">
+        <v>1000</v>
+      </c>
+      <c r="L25">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="7" t="s">
         <v>67</v>
       </c>
       <c r="C26" t="s">
@@ -3157,12 +3684,24 @@
       <c r="H26" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="K26">
+        <v>1000</v>
+      </c>
+      <c r="L26">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="7" t="s">
         <v>68</v>
       </c>
       <c r="C27" t="s">
@@ -3184,12 +3723,24 @@
       <c r="H27" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27" t="b">
+        <v>1</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="K27">
+        <v>1000</v>
+      </c>
+      <c r="L27">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="7" t="s">
         <v>69</v>
       </c>
       <c r="C28" t="s">
@@ -3211,12 +3762,24 @@
       <c r="H28" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28" t="b">
+        <v>1</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="K28">
+        <v>1000</v>
+      </c>
+      <c r="L28">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="7" t="s">
         <v>70</v>
       </c>
       <c r="C29" t="s">
@@ -3238,12 +3801,24 @@
       <c r="H29" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I29" t="b">
+        <v>1</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="K29">
+        <v>1000</v>
+      </c>
+      <c r="L29">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C30" t="s">
@@ -3265,12 +3840,24 @@
       <c r="H30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I30" t="b">
+        <v>1</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="K30">
+        <v>1000</v>
+      </c>
+      <c r="L30">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="7" t="s">
         <v>72</v>
       </c>
       <c r="C31" t="s">
@@ -3292,12 +3879,24 @@
       <c r="H31" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I31" t="b">
+        <v>1</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="K31">
+        <v>1000</v>
+      </c>
+      <c r="L31">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="7" t="s">
         <v>73</v>
       </c>
       <c r="C32" t="s">
@@ -3319,12 +3918,24 @@
       <c r="H32" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I32" t="b">
+        <v>1</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="K32">
+        <v>1000</v>
+      </c>
+      <c r="L32">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="7" t="s">
         <v>74</v>
       </c>
       <c r="C33" t="s">
@@ -3346,12 +3957,24 @@
       <c r="H33" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I33" t="b">
+        <v>1</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="K33">
+        <v>1000</v>
+      </c>
+      <c r="L33">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="7" t="s">
         <v>75</v>
       </c>
       <c r="C34" t="s">
@@ -3373,12 +3996,24 @@
       <c r="H34" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I34" t="b">
+        <v>1</v>
+      </c>
+      <c r="J34" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="K34">
+        <v>1000</v>
+      </c>
+      <c r="L34">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="7" t="s">
         <v>76</v>
       </c>
       <c r="C35" t="s">
@@ -3400,12 +4035,24 @@
       <c r="H35" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I35" t="b">
+        <v>1</v>
+      </c>
+      <c r="J35" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="K35">
+        <v>1000</v>
+      </c>
+      <c r="L35">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="7" t="s">
         <v>77</v>
       </c>
       <c r="C36" t="s">
@@ -3427,12 +4074,24 @@
       <c r="H36" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I36" t="b">
+        <v>1</v>
+      </c>
+      <c r="J36" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="K36">
+        <v>1000</v>
+      </c>
+      <c r="L36">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="7" t="s">
         <v>78</v>
       </c>
       <c r="C37" t="s">
@@ -3454,12 +4113,24 @@
       <c r="H37" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I37" t="b">
+        <v>1</v>
+      </c>
+      <c r="J37" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="K37">
+        <v>1000</v>
+      </c>
+      <c r="L37">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="7" t="s">
         <v>79</v>
       </c>
       <c r="C38" t="s">
@@ -3481,12 +4152,24 @@
       <c r="H38" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I38" t="b">
+        <v>1</v>
+      </c>
+      <c r="J38" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="K38">
+        <v>500</v>
+      </c>
+      <c r="L38">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="7" t="s">
         <v>80</v>
       </c>
       <c r="C39" t="s">
@@ -3503,17 +4186,29 @@
         <v>4</v>
       </c>
       <c r="G39" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="H39" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="I39" t="b">
+        <v>1</v>
+      </c>
+      <c r="J39" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="K39">
+        <v>500</v>
+      </c>
+      <c r="L39">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="7" t="s">
         <v>81</v>
       </c>
       <c r="C40" t="s">
@@ -3535,12 +4230,24 @@
       <c r="H40" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I40" t="b">
+        <v>1</v>
+      </c>
+      <c r="J40" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="K40">
+        <v>500</v>
+      </c>
+      <c r="L40">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="7" t="s">
         <v>82</v>
       </c>
       <c r="C41" t="s">
@@ -3557,17 +4264,29 @@
         <v>4</v>
       </c>
       <c r="G41" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="H41" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="I41" t="b">
+        <v>1</v>
+      </c>
+      <c r="J41" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="K41">
+        <v>500</v>
+      </c>
+      <c r="L41">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="7" t="s">
         <v>83</v>
       </c>
       <c r="C42" t="s">
@@ -3589,12 +4308,24 @@
       <c r="H42" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I42" t="b">
+        <v>1</v>
+      </c>
+      <c r="J42" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="K42">
+        <v>500</v>
+      </c>
+      <c r="L42">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>41</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="7" t="s">
         <v>84</v>
       </c>
       <c r="C43" t="s">
@@ -3611,17 +4342,29 @@
         <v>5</v>
       </c>
       <c r="G43" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="H43" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="I43" t="b">
+        <v>1</v>
+      </c>
+      <c r="J43" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="K43">
+        <v>500</v>
+      </c>
+      <c r="L43">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>42</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="7" t="s">
         <v>85</v>
       </c>
       <c r="C44" t="s">
@@ -3643,12 +4386,24 @@
       <c r="H44" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I44" t="b">
+        <v>1</v>
+      </c>
+      <c r="J44" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="K44">
+        <v>500</v>
+      </c>
+      <c r="L44">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>43</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="7" t="s">
         <v>86</v>
       </c>
       <c r="C45" t="s">
@@ -3665,17 +4420,29 @@
         <v>5</v>
       </c>
       <c r="G45" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="H45" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="I45" t="b">
+        <v>1</v>
+      </c>
+      <c r="J45" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="K45">
+        <v>500</v>
+      </c>
+      <c r="L45">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>44</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="7" t="s">
         <v>87</v>
       </c>
       <c r="C46" t="s">
@@ -3697,12 +4464,24 @@
       <c r="H46" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I46" t="b">
+        <v>1</v>
+      </c>
+      <c r="J46" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="K46">
+        <v>500</v>
+      </c>
+      <c r="L46">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>45</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="7" t="s">
         <v>87</v>
       </c>
       <c r="C47" t="s">
@@ -3724,12 +4503,24 @@
       <c r="H47" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I47" t="b">
+        <v>1</v>
+      </c>
+      <c r="J47" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="K47">
+        <v>500</v>
+      </c>
+      <c r="L47">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>46</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="7" t="s">
         <v>88</v>
       </c>
       <c r="C48" t="s">
@@ -3751,12 +4542,24 @@
       <c r="H48" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I48" t="b">
+        <v>1</v>
+      </c>
+      <c r="J48" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="K48">
+        <v>500</v>
+      </c>
+      <c r="L48">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>47</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="7" t="s">
         <v>89</v>
       </c>
       <c r="C49" t="s">
@@ -3773,17 +4576,29 @@
         <v>6</v>
       </c>
       <c r="G49" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="H49" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="I49" t="b">
+        <v>1</v>
+      </c>
+      <c r="J49" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="K49">
+        <v>500</v>
+      </c>
+      <c r="L49">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>48</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="7" t="s">
         <v>90</v>
       </c>
       <c r="C50" t="s">
@@ -3805,12 +4620,24 @@
       <c r="H50" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I50" t="b">
+        <v>1</v>
+      </c>
+      <c r="J50" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="K50">
+        <v>1000</v>
+      </c>
+      <c r="L50">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>49</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="7" t="s">
         <v>40</v>
       </c>
       <c r="C51" t="s">
@@ -3832,12 +4659,24 @@
       <c r="H51" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I51" t="b">
+        <v>1</v>
+      </c>
+      <c r="J51" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="K51">
+        <v>1000</v>
+      </c>
+      <c r="L51">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>50</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="7" t="s">
         <v>91</v>
       </c>
       <c r="C52" t="s">
@@ -3859,12 +4698,24 @@
       <c r="H52" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I52" t="b">
+        <v>1</v>
+      </c>
+      <c r="J52" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="K52">
+        <v>1000</v>
+      </c>
+      <c r="L52">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>51</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="7" t="s">
         <v>92</v>
       </c>
       <c r="C53" t="s">
@@ -3886,12 +4737,24 @@
       <c r="H53" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I53" t="b">
+        <v>1</v>
+      </c>
+      <c r="J53" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="K53">
+        <v>1000</v>
+      </c>
+      <c r="L53">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>52</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="7" t="s">
         <v>93</v>
       </c>
       <c r="C54" t="s">
@@ -3913,12 +4776,24 @@
       <c r="H54" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I54" t="b">
+        <v>1</v>
+      </c>
+      <c r="J54" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="K54">
+        <v>1000</v>
+      </c>
+      <c r="L54">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>53</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="7" t="s">
         <v>94</v>
       </c>
       <c r="C55" t="s">
@@ -3935,17 +4810,29 @@
         <v>2</v>
       </c>
       <c r="G55" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="H55" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="I55" t="b">
+        <v>1</v>
+      </c>
+      <c r="J55" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="K55">
+        <v>1000</v>
+      </c>
+      <c r="L55">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>54</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="7" t="s">
         <v>95</v>
       </c>
       <c r="C56" t="s">
@@ -3967,12 +4854,24 @@
       <c r="H56" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I56" t="b">
+        <v>1</v>
+      </c>
+      <c r="J56" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="K56">
+        <v>1000</v>
+      </c>
+      <c r="L56">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>55</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C57" t="s">
@@ -3989,17 +4888,29 @@
         <v>2</v>
       </c>
       <c r="G57" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="H57" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="I57" t="b">
+        <v>1</v>
+      </c>
+      <c r="J57" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="K57">
+        <v>1000</v>
+      </c>
+      <c r="L57">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>56</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="7" t="s">
         <v>97</v>
       </c>
       <c r="C58" t="s">
@@ -4021,12 +4932,24 @@
       <c r="H58" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I58" t="b">
+        <v>1</v>
+      </c>
+      <c r="J58" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="K58">
+        <v>1000</v>
+      </c>
+      <c r="L58">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>57</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="7" t="s">
         <v>98</v>
       </c>
       <c r="C59" t="s">
@@ -4043,17 +4966,29 @@
         <v>3</v>
       </c>
       <c r="G59" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="H59" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="I59" t="b">
+        <v>1</v>
+      </c>
+      <c r="J59" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="K59">
+        <v>1000</v>
+      </c>
+      <c r="L59">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>58</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="7" t="s">
         <v>99</v>
       </c>
       <c r="C60" t="s">
@@ -4075,12 +5010,24 @@
       <c r="H60" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I60" t="b">
+        <v>1</v>
+      </c>
+      <c r="J60" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="K60">
+        <v>1000</v>
+      </c>
+      <c r="L60">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>59</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="7" t="s">
         <v>100</v>
       </c>
       <c r="C61" t="s">
@@ -4097,17 +5044,29 @@
         <v>3</v>
       </c>
       <c r="G61" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="H61" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="I61" t="b">
+        <v>1</v>
+      </c>
+      <c r="J61" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="K61">
+        <v>1000</v>
+      </c>
+      <c r="L61">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>60</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="7" t="s">
         <v>101</v>
       </c>
       <c r="C62" t="s">
@@ -4129,12 +5088,24 @@
       <c r="H62" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I62" t="b">
+        <v>1</v>
+      </c>
+      <c r="J62" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="K62">
+        <v>1000</v>
+      </c>
+      <c r="L62">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>61</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="7" t="s">
         <v>102</v>
       </c>
       <c r="C63" t="s">
@@ -4151,17 +5122,29 @@
         <v>4</v>
       </c>
       <c r="G63" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="H63" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="I63" t="b">
+        <v>1</v>
+      </c>
+      <c r="J63" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="K63">
+        <v>1000</v>
+      </c>
+      <c r="L63">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>62</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="7" t="s">
         <v>103</v>
       </c>
       <c r="C64" t="s">
@@ -4183,12 +5166,24 @@
       <c r="H64" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I64" t="b">
+        <v>1</v>
+      </c>
+      <c r="J64" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="K64">
+        <v>1000</v>
+      </c>
+      <c r="L64">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>63</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="7" t="s">
         <v>104</v>
       </c>
       <c r="C65" t="s">
@@ -4205,17 +5200,29 @@
         <v>4</v>
       </c>
       <c r="G65" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="H65" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="I65" t="b">
+        <v>1</v>
+      </c>
+      <c r="J65" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="K65">
+        <v>1000</v>
+      </c>
+      <c r="L65">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>64</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="7" t="s">
         <v>105</v>
       </c>
       <c r="C66" t="s">
@@ -4237,12 +5244,24 @@
       <c r="H66" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I66" t="b">
+        <v>1</v>
+      </c>
+      <c r="J66" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="K66">
+        <v>1000</v>
+      </c>
+      <c r="L66">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>65</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="7" t="s">
         <v>106</v>
       </c>
       <c r="C67" t="s">
@@ -4259,17 +5278,29 @@
         <v>5</v>
       </c>
       <c r="G67" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="H67" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="I67" t="b">
+        <v>1</v>
+      </c>
+      <c r="J67" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="K67">
+        <v>1000</v>
+      </c>
+      <c r="L67">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>66</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="7" t="s">
         <v>107</v>
       </c>
       <c r="C68" t="s">
@@ -4291,12 +5322,24 @@
       <c r="H68" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I68" t="b">
+        <v>1</v>
+      </c>
+      <c r="J68" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="K68">
+        <v>1000</v>
+      </c>
+      <c r="L68">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>67</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="7" t="s">
         <v>108</v>
       </c>
       <c r="C69" t="s">
@@ -4313,17 +5356,29 @@
         <v>5</v>
       </c>
       <c r="G69" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="H69" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="I69" t="b">
+        <v>1</v>
+      </c>
+      <c r="J69" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="K69">
+        <v>1000</v>
+      </c>
+      <c r="L69">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>68</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="7" t="s">
         <v>109</v>
       </c>
       <c r="C70" t="s">
@@ -4345,12 +5400,16 @@
       <c r="H70" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I70" t="b">
+        <v>0</v>
+      </c>
+      <c r="J70" s="7"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>69</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="7" t="s">
         <v>109</v>
       </c>
       <c r="C71" t="s">
@@ -4372,12 +5431,16 @@
       <c r="H71" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I71" t="b">
+        <v>0</v>
+      </c>
+      <c r="J71" s="7"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>70</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="7" t="s">
         <v>110</v>
       </c>
       <c r="C72" t="s">
@@ -4399,12 +5462,16 @@
       <c r="H72" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I72" t="b">
+        <v>0</v>
+      </c>
+      <c r="J72" s="7"/>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>71</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="7" t="s">
         <v>111</v>
       </c>
       <c r="C73" t="s">
@@ -4425,6 +5492,9 @@
       </c>
       <c r="H73" t="s">
         <v>39</v>
+      </c>
+      <c r="I73" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4440,7 +5510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9175E36E-43BA-5E42-B7A5-8B1A23A27503}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+    <sheetView zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated 1-channel m3 config
</commit_message>
<xml_diff>
--- a/model_config.xlsx
+++ b/model_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asafsilman/Desktop/GENG5511/GalaxyEnvironmentAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE6884F-A26F-E746-80D8-6D9891C075D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382095AB-01B6-EB48-8BB8-F8A8A6506B35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" activeTab="1" xr2:uid="{DA573336-42C9-534D-A3C9-C8C047CC3E2B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="190">
   <si>
     <t>modelName</t>
   </si>
@@ -596,6 +596,15 @@
   </si>
   <si>
     <t>m6</t>
+  </si>
+  <si>
+    <t>e6c64921e0d83fbd317d7182e7631d6527c97e0675ca7e8a54b9f8f1028b693c</t>
+  </si>
+  <si>
+    <t>ebbe11c1eee9b05ce6535d50c93c3f8aec60d9f2421167c71dec821e12a56c68</t>
+  </si>
+  <si>
+    <t>a87d18e9f499b51ddd5cf00fd96432f3022c2a931f7520b23fc68f8b78a369f7</t>
   </si>
 </sst>
 </file>
@@ -1113,7 +1122,7 @@
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2686,7 +2695,7 @@
   <dimension ref="A1:L73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="J68" sqref="J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5419,9 +5428,17 @@
         <v>35</v>
       </c>
       <c r="I70" t="b">
-        <v>0</v>
-      </c>
-      <c r="J70" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="J70" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="K70">
+        <v>1000</v>
+      </c>
+      <c r="L70">
+        <v>1000</v>
+      </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71">
@@ -5450,9 +5467,17 @@
         <v>35</v>
       </c>
       <c r="I71" t="b">
-        <v>0</v>
-      </c>
-      <c r="J71" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="J71" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="K71">
+        <v>1000</v>
+      </c>
+      <c r="L71">
+        <v>1000</v>
+      </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72">
@@ -5481,9 +5506,17 @@
         <v>35</v>
       </c>
       <c r="I72" t="b">
-        <v>0</v>
-      </c>
-      <c r="J72" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="J72" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="K72">
+        <v>1000</v>
+      </c>
+      <c r="L72">
+        <v>1000</v>
+      </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73">
@@ -5506,13 +5539,22 @@
         <v>186</v>
       </c>
       <c r="G73" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="H73" t="s">
-        <v>35</v>
+        <v>152</v>
       </c>
       <c r="I73" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J73" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="K73">
+        <v>1000</v>
+      </c>
+      <c r="L73">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new model data set code
</commit_message>
<xml_diff>
--- a/model_config.xlsx
+++ b/model_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asafsilman/Desktop/GENG5511/GalaxyEnvironmentAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382095AB-01B6-EB48-8BB8-F8A8A6506B35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4074CC42-0C10-A044-8765-475BE917D0DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" activeTab="1" xr2:uid="{DA573336-42C9-534D-A3C9-C8C047CC3E2B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" xr2:uid="{DA573336-42C9-534D-A3C9-C8C047CC3E2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="1" r:id="rId1"/>
@@ -790,7 +790,21 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BBA15079-BA5C-4347-AB18-D63DE85A40E7}" name="Table1" displayName="Table1" ref="A1:L73" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:L73" xr:uid="{1608FF67-3914-5949-96DC-606C50EA2E4D}"/>
+  <autoFilter ref="A1:L73" xr:uid="{1608FF67-3914-5949-96DC-606C50EA2E4D}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="gas_density"/>
+        <filter val="star_density"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="5">
+      <filters>
+        <filter val="m1"/>
+        <filter val="m2"/>
+        <filter val="m3"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{AE589D12-F9F2-7E46-B3F1-011FE87BB9E7}" name="dataId"/>
     <tableColumn id="2" xr3:uid="{86A820C4-44CA-F647-A338-3C42F8D54CAF}" name="dataFile" dataDxfId="2"/>
@@ -1121,8 +1135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F969F3E7-5EBB-B140-87B5-F57642023AAB}">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2694,8 +2708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A15A60-C633-ED48-8690-686D42EE8C24}">
   <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J68" sqref="J68"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B4" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2788,7 +2802,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2866,7 +2880,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2944,7 +2958,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3022,7 +3036,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3100,7 +3114,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3178,7 +3192,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3217,7 +3231,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3256,7 +3270,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3295,7 +3309,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -3334,7 +3348,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -3373,7 +3387,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -3412,7 +3426,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -3451,7 +3465,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -3490,7 +3504,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -3529,7 +3543,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -3568,7 +3582,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -3607,7 +3621,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -3646,7 +3660,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -3724,7 +3738,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -3802,7 +3816,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -3880,7 +3894,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -3958,7 +3972,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
@@ -4036,7 +4050,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
@@ -4114,7 +4128,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
@@ -4153,7 +4167,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
@@ -4192,7 +4206,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
@@ -4231,7 +4245,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
@@ -4270,7 +4284,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
@@ -4309,7 +4323,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
@@ -4348,7 +4362,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>41</v>
       </c>
@@ -4387,7 +4401,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>42</v>
       </c>
@@ -4426,7 +4440,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>43</v>
       </c>
@@ -4465,7 +4479,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>44</v>
       </c>
@@ -4504,7 +4518,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>45</v>
       </c>
@@ -4543,7 +4557,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>46</v>
       </c>
@@ -4582,7 +4596,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>47</v>
       </c>
@@ -4660,7 +4674,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>49</v>
       </c>
@@ -4738,7 +4752,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>51</v>
       </c>
@@ -4816,7 +4830,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>53</v>
       </c>
@@ -4894,7 +4908,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>55</v>
       </c>
@@ -4972,7 +4986,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>57</v>
       </c>
@@ -5050,7 +5064,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>59</v>
       </c>
@@ -5089,7 +5103,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>60</v>
       </c>
@@ -5128,7 +5142,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>61</v>
       </c>
@@ -5167,7 +5181,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>62</v>
       </c>
@@ -5206,7 +5220,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>63</v>
       </c>
@@ -5245,7 +5259,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>64</v>
       </c>
@@ -5284,7 +5298,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>65</v>
       </c>
@@ -5323,7 +5337,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>66</v>
       </c>
@@ -5362,7 +5376,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>67</v>
       </c>
@@ -5401,7 +5415,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>68</v>
       </c>
@@ -5440,7 +5454,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>69</v>
       </c>
@@ -5479,7 +5493,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>70</v>
       </c>
@@ -5518,7 +5532,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>71</v>
       </c>

</xml_diff>

<commit_message>
Added m4a, m7, m8 and m9 data to model config for RPS, updated erronious data files
</commit_message>
<xml_diff>
--- a/model_config.xlsx
+++ b/model_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asafsilman/Desktop/GENG5511/GalaxyEnvironmentAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4074CC42-0C10-A044-8765-475BE917D0DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2FAF1B-AF3F-034E-AD12-98392051772F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" xr2:uid="{DA573336-42C9-534D-A3C9-C8C047CC3E2B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" activeTab="1" xr2:uid="{DA573336-42C9-534D-A3C9-C8C047CC3E2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="226">
   <si>
     <t>modelName</t>
   </si>
@@ -605,6 +605,114 @@
   </si>
   <si>
     <t>a87d18e9f499b51ddd5cf00fd96432f3022c2a931f7520b23fc68f8b78a369f7</t>
+  </si>
+  <si>
+    <t>A.r.m7.dir.tar.gz</t>
+  </si>
+  <si>
+    <t>A.rs.m7.dir.tar.gz</t>
+  </si>
+  <si>
+    <t>A.rs.m7v.dir.tar.gz</t>
+  </si>
+  <si>
+    <t>A.r.m8.dir.tar.gz</t>
+  </si>
+  <si>
+    <t>A.rs.m8.dir.tar.gz</t>
+  </si>
+  <si>
+    <t>A.rs.m8v.dir.tar.gz</t>
+  </si>
+  <si>
+    <t>A.r.m9.dir.tar.gz</t>
+  </si>
+  <si>
+    <t>A.rs.m9.dir.tar.gz</t>
+  </si>
+  <si>
+    <t>A.rs.m9v.dir.tar.gz</t>
+  </si>
+  <si>
+    <t>m8</t>
+  </si>
+  <si>
+    <t>m9</t>
+  </si>
+  <si>
+    <t>m4a</t>
+  </si>
+  <si>
+    <t>dataSet_m4a</t>
+  </si>
+  <si>
+    <t>dataSet_m7</t>
+  </si>
+  <si>
+    <t>dataSet_m8</t>
+  </si>
+  <si>
+    <t>e0d573a2c809f8787284ba206cd2086d162975229186840a37bc3bc9b1a331cd</t>
+  </si>
+  <si>
+    <t>A.r.m6v.dir.tar.gz</t>
+  </si>
+  <si>
+    <t>A.r.m7v.dir.tar.gz</t>
+  </si>
+  <si>
+    <t>A.r.m8v.dir.tar.gz</t>
+  </si>
+  <si>
+    <t>A.r.m9v.dir.tar.gz</t>
+  </si>
+  <si>
+    <t>1c8ee3156094fa7819d206d619699af0cf9de4cc43714b3921a2a6b3b4bdd901</t>
+  </si>
+  <si>
+    <t>426df618f3446e66265bc2379547225af3c051c5212c606d2a18866072ed1c78</t>
+  </si>
+  <si>
+    <t>2e52e24f05b3e5e7f35b27dc2fc9f20f73593b643263e7145b6c1781fe53a091</t>
+  </si>
+  <si>
+    <t>1cf03636eae31b48ee49381c6a770adf914d2cb0631476b459cf73a16e17e790</t>
+  </si>
+  <si>
+    <t>97d9e049d39c5212c3ede6162adbb74930ed168953215d279edf9f35ec016452</t>
+  </si>
+  <si>
+    <t>00b821cff097d124a22ce12e71a5f4e927814f33c06f2e900b4e3b4c0811f901</t>
+  </si>
+  <si>
+    <t>16a2eacb9f3f50a5517870c29939ddc6b695af2e58bd0eaaec8b775664c26747</t>
+  </si>
+  <si>
+    <t>4a48d19586664ce9c9222c679deeb284a7e285207a430be169176eafeb8b2e4f</t>
+  </si>
+  <si>
+    <t>1e5b66b38c0aa1cd91f3514fd3d2e9fb37e5a5c361d410790f434c68916a8874</t>
+  </si>
+  <si>
+    <t>fde37766f524529379762ff1071c7ad99663e6e8fcc578b4352485fae3480116</t>
+  </si>
+  <si>
+    <t>fbb1b8ee3b14535cf27433486da42a229b4b6fc22f666d1c96ad310e436b826e</t>
+  </si>
+  <si>
+    <t>A.i.m6v.dir.tar.gz</t>
+  </si>
+  <si>
+    <t>b0b81e3a2bb881ca0096ec452efe592998248a9b5648d36223c87e72ea8103fe</t>
+  </si>
+  <si>
+    <t>0cfa3cc8f80647227caf8708002ba10c2e8a997f10a2c9195dc26418fa36b5ce</t>
+  </si>
+  <si>
+    <t>A.t.m6v.dir.tar.gz</t>
+  </si>
+  <si>
+    <t>7f60221c52e74c29630b1a8d206fa4d0d1b7af9b757a333a8fb91f3049d2e908</t>
   </si>
 </sst>
 </file>
@@ -671,7 +779,30 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="15">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -730,19 +861,6 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -757,59 +875,48 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BFE53D84-975D-9E44-A5C0-0D53C58F4B56}" name="Table3" displayName="Table3" ref="A1:Q31" totalsRowShown="0">
-  <autoFilter ref="A1:Q31" xr:uid="{CC0FBD37-8587-624E-8633-B9595665FD07}"/>
-  <tableColumns count="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BFE53D84-975D-9E44-A5C0-0D53C58F4B56}" name="Table3" displayName="Table3" ref="A1:T31" totalsRowShown="0">
+  <autoFilter ref="A1:T31" xr:uid="{CC0FBD37-8587-624E-8633-B9595665FD07}"/>
+  <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{703C2328-6727-224A-92DA-FB21A475BF4C}" name="modelId"/>
     <tableColumn id="5" xr3:uid="{091AFF89-BAE7-674D-85D8-5FA5B7DAF36C}" name="modelAltName"/>
-    <tableColumn id="6" xr3:uid="{9243668A-FEFC-2A44-85FD-E9850DCD3F13}" name="modelName" dataDxfId="12">
+    <tableColumn id="6" xr3:uid="{9243668A-FEFC-2A44-85FD-E9850DCD3F13}" name="modelName" dataDxfId="14">
       <calculatedColumnFormula>_xlfn.CONCAT(Table3[[#This Row],[numChannels]],"_channel_",Table3[[#This Row],[modelType]],"_", Table3[[#This Row],[_modelNameString]], "_", Table3[[#This Row],[_modelDataString]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{E6DF2D56-96C3-AF43-9D19-75691A5B5160}" name="_modelNameString" dataDxfId="11">
+    <tableColumn id="20" xr3:uid="{E6DF2D56-96C3-AF43-9D19-75691A5B5160}" name="_modelNameString" dataDxfId="13">
       <calculatedColumnFormula>_xlfn.CONCAT(Table3[[#This Row],[channel1]], IF(Table3[[#This Row],[channel2]]&lt;&gt;"", _xlfn.CONCAT("_",Table3[[#This Row],[channel2]], IF(Table3[[#This Row],[channel3]]&lt;&gt;"", _xlfn.CONCAT("_", Table3[[#This Row],[channel3]]), ""), ""), ""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{25197AF6-7EB6-9344-B947-E907FA36108D}" name="_modelDataString" dataDxfId="10">
-      <calculatedColumnFormula>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</calculatedColumnFormula>
+    <tableColumn id="21" xr3:uid="{25197AF6-7EB6-9344-B947-E907FA36108D}" name="_modelDataString" dataDxfId="0">
+      <calculatedColumnFormula>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{A721B211-0E17-F640-A300-BE3E08E93596}" name="modelType" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{4347DEF6-17C0-3F43-802E-86E8674A6FB3}" name="numChannels" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{3B4B9348-11DD-394A-9D6A-D4850CC40194}" name="channel1" dataDxfId="7"/>
-    <tableColumn id="14" xr3:uid="{B526A24F-2ECC-0442-9CEB-DA811FF165E2}" name="channel2" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{0052B57A-E822-0B40-8C1E-8D026B8A57CC}" name="channel3" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{7E2B00ED-F5EB-4648-9E53-8AB3EC8A396B}" name="channel4" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{A721B211-0E17-F640-A300-BE3E08E93596}" name="modelType" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{4347DEF6-17C0-3F43-802E-86E8674A6FB3}" name="numChannels" dataDxfId="11"/>
+    <tableColumn id="13" xr3:uid="{3B4B9348-11DD-394A-9D6A-D4850CC40194}" name="channel1" dataDxfId="10"/>
+    <tableColumn id="14" xr3:uid="{B526A24F-2ECC-0442-9CEB-DA811FF165E2}" name="channel2" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{0052B57A-E822-0B40-8C1E-8D026B8A57CC}" name="channel3" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{7E2B00ED-F5EB-4648-9E53-8AB3EC8A396B}" name="channel4" dataDxfId="7"/>
     <tableColumn id="9" xr3:uid="{712BD42A-DEBB-2545-A3FE-8F98C541BB5F}" name="dataSet_m1"/>
     <tableColumn id="10" xr3:uid="{1C7EA2DE-42E0-4949-B9B8-64BD2A71AC95}" name="dataSet_m2"/>
     <tableColumn id="11" xr3:uid="{82D55CF4-DECF-6844-ABEC-7EC6D1BC5DA6}" name="dataSet_m3"/>
-    <tableColumn id="15" xr3:uid="{B446571A-5D1D-5F4D-AA88-2C1B2061FBF2}" name="dataSet_m4"/>
+    <tableColumn id="8" xr3:uid="{807E58FC-4F1A-7E43-859F-25EA81465A50}" name="dataSet_m4"/>
+    <tableColumn id="15" xr3:uid="{B446571A-5D1D-5F4D-AA88-2C1B2061FBF2}" name="dataSet_m4a"/>
     <tableColumn id="16" xr3:uid="{DA289666-C113-7446-8094-641BEE34B814}" name="dataSet_m5"/>
     <tableColumn id="17" xr3:uid="{EAB20F55-7FD9-224C-A3DB-181D5CB1A345}" name="dataSet_m6"/>
+    <tableColumn id="12" xr3:uid="{D0D85B70-32C3-1546-9D25-48EF6AA9A2E2}" name="dataSet_m7"/>
+    <tableColumn id="18" xr3:uid="{36F61E23-086F-BD45-812C-CAA7CE0D0D34}" name="dataSet_m8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BBA15079-BA5C-4347-AB18-D63DE85A40E7}" name="Table1" displayName="Table1" ref="A1:L73" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:L73" xr:uid="{1608FF67-3914-5949-96DC-606C50EA2E4D}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="gas_density"/>
-        <filter val="star_density"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="5">
-      <filters>
-        <filter val="m1"/>
-        <filter val="m2"/>
-        <filter val="m3"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BBA15079-BA5C-4347-AB18-D63DE85A40E7}" name="Table1" displayName="Table1" ref="A1:L85" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:L85" xr:uid="{1608FF67-3914-5949-96DC-606C50EA2E4D}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{AE589D12-F9F2-7E46-B3F1-011FE87BB9E7}" name="dataId"/>
-    <tableColumn id="2" xr3:uid="{86A820C4-44CA-F647-A338-3C42F8D54CAF}" name="dataFile" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{86A820C4-44CA-F647-A338-3C42F8D54CAF}" name="dataFile" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{8CB7439C-328A-4840-8650-53C68739CB52}" name="dataLabel"/>
-    <tableColumn id="6" xr3:uid="{20416ED2-C6CE-DB4D-BCD0-4920296FFAB5}" name="dataLabelValue" dataDxfId="1">
+    <tableColumn id="6" xr3:uid="{20416ED2-C6CE-DB4D-BCD0-4920296FFAB5}" name="dataLabelValue" dataDxfId="4">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{ECFC63C3-8324-5B40-8261-525DCDBB1D77}" name="dataSimType"/>
@@ -817,7 +924,7 @@
     <tableColumn id="7" xr3:uid="{A34CD7B0-6947-5A42-AD6C-DDCF954D6599}" name="imageFileName"/>
     <tableColumn id="8" xr3:uid="{4E77CFD9-0959-1946-94BB-C03C9823FFCF}" name="labelFileName"/>
     <tableColumn id="10" xr3:uid="{B5582984-20BB-B04C-ACD1-B32B5C014342}" name="fileAvailable"/>
-    <tableColumn id="9" xr3:uid="{8E67EC6E-99AC-7043-8F51-B1C73A2D564B}" name="fileHash" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{8E67EC6E-99AC-7043-8F51-B1C73A2D564B}" name="fileHash" dataDxfId="3"/>
     <tableColumn id="11" xr3:uid="{38F53538-5DB0-E34C-B916-D0BD7FD2CC71}" name="imageFileNumRows"/>
     <tableColumn id="12" xr3:uid="{E263E244-E409-B344-BD21-61A040BA1A1C}" name="labelFileNumRows"/>
   </tableColumns>
@@ -1133,10 +1240,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F969F3E7-5EBB-B140-87B5-F57642023AAB}">
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1145,15 +1252,18 @@
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="69" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="60.33203125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" customWidth="1"/>
+    <col min="16" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1200,13 +1310,22 @@
         <v>8</v>
       </c>
       <c r="P1" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q1" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S1" t="s">
+        <v>203</v>
+      </c>
+      <c r="T1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1219,7 +1338,7 @@
         <v>gas_density</v>
       </c>
       <c r="E2" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -1252,8 +1371,17 @@
       <c r="Q2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S2" t="b">
+        <v>0</v>
+      </c>
+      <c r="T2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1266,7 +1394,7 @@
         <v>gas_kinematics</v>
       </c>
       <c r="E3" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1299,8 +1427,17 @@
       <c r="Q3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S3" t="b">
+        <v>0</v>
+      </c>
+      <c r="T3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1313,7 +1450,7 @@
         <v>star_density</v>
       </c>
       <c r="E4" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -1346,8 +1483,17 @@
       <c r="Q4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R4" t="b">
+        <v>0</v>
+      </c>
+      <c r="S4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1360,7 +1506,7 @@
         <v>star_kinematics</v>
       </c>
       <c r="E5" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -1393,8 +1539,17 @@
       <c r="Q5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R5" t="b">
+        <v>0</v>
+      </c>
+      <c r="S5" t="b">
+        <v>0</v>
+      </c>
+      <c r="T5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1407,7 +1562,7 @@
         <v>gas_density_star_density</v>
       </c>
       <c r="E6" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -1442,8 +1597,17 @@
       <c r="Q6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R6" t="b">
+        <v>0</v>
+      </c>
+      <c r="S6" t="b">
+        <v>0</v>
+      </c>
+      <c r="T6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1456,7 +1620,7 @@
         <v>gas_density_star_kinematics</v>
       </c>
       <c r="E7" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -1491,8 +1655,17 @@
       <c r="Q7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R7" t="b">
+        <v>0</v>
+      </c>
+      <c r="S7" t="b">
+        <v>0</v>
+      </c>
+      <c r="T7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1505,7 +1678,7 @@
         <v>gas_kinematics_star_density</v>
       </c>
       <c r="E8" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -1540,8 +1713,17 @@
       <c r="Q8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R8" t="b">
+        <v>0</v>
+      </c>
+      <c r="S8" t="b">
+        <v>0</v>
+      </c>
+      <c r="T8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1554,7 +1736,7 @@
         <v>gas_kinematics_star_kinematics</v>
       </c>
       <c r="E9" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -1589,8 +1771,17 @@
       <c r="Q9" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R9" t="b">
+        <v>0</v>
+      </c>
+      <c r="S9" t="b">
+        <v>0</v>
+      </c>
+      <c r="T9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1603,7 +1794,7 @@
         <v>gas_density_gas_kinematics</v>
       </c>
       <c r="E10" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -1638,8 +1829,17 @@
       <c r="Q10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R10" t="b">
+        <v>0</v>
+      </c>
+      <c r="S10" t="b">
+        <v>0</v>
+      </c>
+      <c r="T10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1652,7 +1852,7 @@
         <v>star_density_star_kinematics</v>
       </c>
       <c r="E11" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F11" s="1" t="s">
@@ -1687,8 +1887,17 @@
       <c r="Q11" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R11" t="b">
+        <v>0</v>
+      </c>
+      <c r="S11" t="b">
+        <v>0</v>
+      </c>
+      <c r="T11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1701,7 +1910,7 @@
         <v>gas_density_gas_kinematics_star_density</v>
       </c>
       <c r="E12" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -1738,8 +1947,17 @@
       <c r="Q12" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R12" t="b">
+        <v>0</v>
+      </c>
+      <c r="S12" t="b">
+        <v>0</v>
+      </c>
+      <c r="T12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1752,7 +1970,7 @@
         <v>gas_density_gas_kinematics_star_density</v>
       </c>
       <c r="E13" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F13" s="1" t="s">
@@ -1789,8 +2007,17 @@
       <c r="Q13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R13" t="b">
+        <v>0</v>
+      </c>
+      <c r="S13" t="b">
+        <v>0</v>
+      </c>
+      <c r="T13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1803,7 +2030,7 @@
         <v>gas_density_star_density_star_kinematics</v>
       </c>
       <c r="E14" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F14" s="1" t="s">
@@ -1840,8 +2067,17 @@
       <c r="Q14" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R14" t="b">
+        <v>0</v>
+      </c>
+      <c r="S14" t="b">
+        <v>0</v>
+      </c>
+      <c r="T14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1854,7 +2090,7 @@
         <v>gas_kinematics_star_density_star_kinematics</v>
       </c>
       <c r="E15" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F15" s="1" t="s">
@@ -1891,8 +2127,17 @@
       <c r="Q15" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R15" t="b">
+        <v>0</v>
+      </c>
+      <c r="S15" t="b">
+        <v>0</v>
+      </c>
+      <c r="T15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1908,7 +2153,7 @@
         <v>gas_density_gas_kinematics_star_density</v>
       </c>
       <c r="E16" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F16" s="1" t="s">
@@ -1947,8 +2192,17 @@
       <c r="Q16" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R16" t="b">
+        <v>0</v>
+      </c>
+      <c r="S16" t="b">
+        <v>0</v>
+      </c>
+      <c r="T16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1961,7 +2215,7 @@
         <v>gas_density</v>
       </c>
       <c r="E17" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F17" s="1" t="s">
@@ -1994,8 +2248,17 @@
       <c r="Q17" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R17" t="b">
+        <v>0</v>
+      </c>
+      <c r="S17" t="b">
+        <v>0</v>
+      </c>
+      <c r="T17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2008,7 +2271,7 @@
         <v>gas_kinematics</v>
       </c>
       <c r="E18" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F18" s="1" t="s">
@@ -2041,8 +2304,17 @@
       <c r="Q18" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R18" t="b">
+        <v>0</v>
+      </c>
+      <c r="S18" t="b">
+        <v>0</v>
+      </c>
+      <c r="T18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2055,7 +2327,7 @@
         <v>star_density</v>
       </c>
       <c r="E19" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F19" s="1" t="s">
@@ -2088,8 +2360,17 @@
       <c r="Q19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R19" t="b">
+        <v>0</v>
+      </c>
+      <c r="S19" t="b">
+        <v>0</v>
+      </c>
+      <c r="T19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2102,7 +2383,7 @@
         <v>star_kinematics</v>
       </c>
       <c r="E20" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F20" s="1" t="s">
@@ -2135,8 +2416,17 @@
       <c r="Q20" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R20" t="b">
+        <v>0</v>
+      </c>
+      <c r="S20" t="b">
+        <v>0</v>
+      </c>
+      <c r="T20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2149,7 +2439,7 @@
         <v>gas_density_star_density</v>
       </c>
       <c r="E21" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F21" s="1" t="s">
@@ -2184,8 +2474,17 @@
       <c r="Q21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R21" t="b">
+        <v>0</v>
+      </c>
+      <c r="S21" t="b">
+        <v>0</v>
+      </c>
+      <c r="T21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2198,7 +2497,7 @@
         <v>gas_density_star_kinematics</v>
       </c>
       <c r="E22" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F22" s="1" t="s">
@@ -2233,8 +2532,17 @@
       <c r="Q22" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R22" t="b">
+        <v>0</v>
+      </c>
+      <c r="S22" t="b">
+        <v>0</v>
+      </c>
+      <c r="T22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2247,7 +2555,7 @@
         <v>gas_kinematics_star_density</v>
       </c>
       <c r="E23" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F23" s="1" t="s">
@@ -2282,8 +2590,17 @@
       <c r="Q23" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R23" t="b">
+        <v>0</v>
+      </c>
+      <c r="S23" t="b">
+        <v>0</v>
+      </c>
+      <c r="T23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2296,7 +2613,7 @@
         <v>gas_kinematics_star_kinematics</v>
       </c>
       <c r="E24" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F24" s="1" t="s">
@@ -2331,8 +2648,17 @@
       <c r="Q24" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R24" t="b">
+        <v>0</v>
+      </c>
+      <c r="S24" t="b">
+        <v>0</v>
+      </c>
+      <c r="T24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2345,7 +2671,7 @@
         <v>gas_density_gas_kinematics</v>
       </c>
       <c r="E25" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F25" s="1" t="s">
@@ -2380,8 +2706,17 @@
       <c r="Q25" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R25" t="b">
+        <v>0</v>
+      </c>
+      <c r="S25" t="b">
+        <v>0</v>
+      </c>
+      <c r="T25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2394,7 +2729,7 @@
         <v>star_density_star_kinematics</v>
       </c>
       <c r="E26" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F26" s="1" t="s">
@@ -2429,8 +2764,17 @@
       <c r="Q26" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R26" t="b">
+        <v>0</v>
+      </c>
+      <c r="S26" t="b">
+        <v>0</v>
+      </c>
+      <c r="T26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2443,7 +2787,7 @@
         <v>gas_density_gas_kinematics_star_density</v>
       </c>
       <c r="E27" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F27" s="1" t="s">
@@ -2480,8 +2824,17 @@
       <c r="Q27" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R27" t="b">
+        <v>0</v>
+      </c>
+      <c r="S27" t="b">
+        <v>0</v>
+      </c>
+      <c r="T27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2494,7 +2847,7 @@
         <v>gas_density_gas_kinematics_star_density</v>
       </c>
       <c r="E28" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F28" s="1" t="s">
@@ -2531,8 +2884,17 @@
       <c r="Q28" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R28" t="b">
+        <v>0</v>
+      </c>
+      <c r="S28" t="b">
+        <v>0</v>
+      </c>
+      <c r="T28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2545,7 +2907,7 @@
         <v>gas_density_star_density_star_kinematics</v>
       </c>
       <c r="E29" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F29" s="1" t="s">
@@ -2582,8 +2944,17 @@
       <c r="Q29" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R29" t="b">
+        <v>0</v>
+      </c>
+      <c r="S29" t="b">
+        <v>0</v>
+      </c>
+      <c r="T29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2596,7 +2967,7 @@
         <v>gas_kinematics_star_density_star_kinematics</v>
       </c>
       <c r="E30" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F30" s="1" t="s">
@@ -2633,8 +3004,17 @@
       <c r="Q30" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R30" t="b">
+        <v>0</v>
+      </c>
+      <c r="S30" t="b">
+        <v>0</v>
+      </c>
+      <c r="T30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2650,7 +3030,7 @@
         <v>gas_density_gas_kinematics_star_density</v>
       </c>
       <c r="E31" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F31" s="1" t="s">
@@ -2689,11 +3069,25 @@
       <c r="Q31" t="b">
         <v>0</v>
       </c>
+      <c r="R31" t="b">
+        <v>0</v>
+      </c>
+      <c r="S31" t="b">
+        <v>0</v>
+      </c>
+      <c r="T31" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="L2:Q31">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+  <conditionalFormatting sqref="L2:N31 P2:T31">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:O31">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2706,10 +3100,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A15A60-C633-ED48-8690-686D42EE8C24}">
-  <dimension ref="A1:L73"/>
+  <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B4" sqref="B2:B4"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L58" sqref="L58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2802,7 +3196,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2880,7 +3274,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2958,7 +3352,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3036,7 +3430,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3114,7 +3508,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3192,7 +3586,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3231,7 +3625,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3270,7 +3664,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3309,7 +3703,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -3348,7 +3742,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -3387,7 +3781,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -3426,7 +3820,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -3465,7 +3859,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -3504,7 +3898,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -3543,7 +3937,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -3582,12 +3976,12 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>60</v>
+        <v>224</v>
       </c>
       <c r="C23" t="s">
         <v>25</v>
@@ -3603,16 +3997,16 @@
         <v>186</v>
       </c>
       <c r="G23" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="H23" t="s">
-        <v>35</v>
+        <v>152</v>
       </c>
       <c r="I23" t="b">
         <v>1</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>157</v>
+        <v>225</v>
       </c>
       <c r="K23">
         <v>1000</v>
@@ -3621,7 +4015,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -3660,7 +4054,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -3738,7 +4132,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -3816,7 +4210,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -3894,7 +4288,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -3972,7 +4366,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
@@ -4050,7 +4444,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
@@ -4128,7 +4522,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
@@ -4167,7 +4561,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
@@ -4185,7 +4579,7 @@
         <v>11</v>
       </c>
       <c r="F38" t="s">
-        <v>184</v>
+        <v>201</v>
       </c>
       <c r="G38" t="s">
         <v>34</v>
@@ -4206,7 +4600,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
@@ -4224,7 +4618,7 @@
         <v>14</v>
       </c>
       <c r="F39" t="s">
-        <v>184</v>
+        <v>201</v>
       </c>
       <c r="G39" t="s">
         <v>151</v>
@@ -4245,7 +4639,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
@@ -4263,7 +4657,7 @@
         <v>12</v>
       </c>
       <c r="F40" t="s">
-        <v>184</v>
+        <v>201</v>
       </c>
       <c r="G40" t="s">
         <v>34</v>
@@ -4284,7 +4678,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
@@ -4302,7 +4696,7 @@
         <v>13</v>
       </c>
       <c r="F41" t="s">
-        <v>184</v>
+        <v>201</v>
       </c>
       <c r="G41" t="s">
         <v>151</v>
@@ -4323,7 +4717,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
@@ -4362,7 +4756,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>41</v>
       </c>
@@ -4401,7 +4795,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>42</v>
       </c>
@@ -4440,7 +4834,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>43</v>
       </c>
@@ -4479,7 +4873,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>44</v>
       </c>
@@ -4518,12 +4912,12 @@
         <v>500</v>
       </c>
     </row>
-    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>45</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>83</v>
+        <v>206</v>
       </c>
       <c r="C47" t="s">
         <v>26</v>
@@ -4539,16 +4933,16 @@
         <v>186</v>
       </c>
       <c r="G47" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="H47" t="s">
-        <v>35</v>
+        <v>152</v>
       </c>
       <c r="I47" t="b">
         <v>1</v>
       </c>
       <c r="J47" s="7" t="s">
-        <v>141</v>
+        <v>210</v>
       </c>
       <c r="K47">
         <v>500</v>
@@ -4557,7 +4951,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>46</v>
       </c>
@@ -4596,7 +4990,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>47</v>
       </c>
@@ -4640,20 +5034,20 @@
         <v>48</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>86</v>
+        <v>190</v>
       </c>
       <c r="C50" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D50" s="5">
         <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E50" t="s">
         <v>11</v>
       </c>
       <c r="F50" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="G50" t="s">
         <v>34</v>
@@ -4665,7 +5059,7 @@
         <v>1</v>
       </c>
       <c r="J50" s="7" t="s">
-        <v>144</v>
+        <v>205</v>
       </c>
       <c r="K50">
         <v>1000</v>
@@ -4674,37 +5068,37 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>49</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>36</v>
+        <v>207</v>
       </c>
       <c r="C51" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D51" s="5">
         <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E51" t="s">
         <v>14</v>
       </c>
       <c r="F51" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="G51" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="H51" t="s">
-        <v>35</v>
+        <v>152</v>
       </c>
       <c r="I51" t="b">
         <v>1</v>
       </c>
       <c r="J51" s="7" t="s">
-        <v>145</v>
+        <v>211</v>
       </c>
       <c r="K51">
         <v>1000</v>
@@ -4718,20 +5112,20 @@
         <v>50</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>87</v>
+        <v>191</v>
       </c>
       <c r="C52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D52" s="5">
         <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E52" t="s">
         <v>12</v>
       </c>
       <c r="F52" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="G52" t="s">
         <v>34</v>
@@ -4743,7 +5137,7 @@
         <v>1</v>
       </c>
       <c r="J52" s="7" t="s">
-        <v>146</v>
+        <v>212</v>
       </c>
       <c r="K52">
         <v>1000</v>
@@ -4752,37 +5146,37 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>51</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>88</v>
+        <v>192</v>
       </c>
       <c r="C53" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D53" s="5">
         <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E53" t="s">
         <v>13</v>
       </c>
       <c r="F53" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="G53" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="H53" t="s">
-        <v>35</v>
+        <v>152</v>
       </c>
       <c r="I53" t="b">
         <v>1</v>
       </c>
       <c r="J53" s="7" t="s">
-        <v>147</v>
+        <v>213</v>
       </c>
       <c r="K53">
         <v>1000</v>
@@ -4796,20 +5190,20 @@
         <v>52</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>89</v>
+        <v>193</v>
       </c>
       <c r="C54" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D54" s="5">
         <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E54" t="s">
         <v>11</v>
       </c>
       <c r="F54" t="s">
-        <v>182</v>
+        <v>199</v>
       </c>
       <c r="G54" t="s">
         <v>34</v>
@@ -4821,7 +5215,7 @@
         <v>1</v>
       </c>
       <c r="J54" s="7" t="s">
-        <v>164</v>
+        <v>214</v>
       </c>
       <c r="K54">
         <v>1000</v>
@@ -4830,25 +5224,25 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>53</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>90</v>
+        <v>208</v>
       </c>
       <c r="C55" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D55" s="5">
         <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E55" t="s">
         <v>14</v>
       </c>
       <c r="F55" t="s">
-        <v>182</v>
+        <v>199</v>
       </c>
       <c r="G55" t="s">
         <v>151</v>
@@ -4860,7 +5254,7 @@
         <v>1</v>
       </c>
       <c r="J55" s="7" t="s">
-        <v>148</v>
+        <v>215</v>
       </c>
       <c r="K55">
         <v>1000</v>
@@ -4874,20 +5268,20 @@
         <v>54</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>91</v>
+        <v>194</v>
       </c>
       <c r="C56" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D56" s="5">
         <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E56" t="s">
         <v>12</v>
       </c>
       <c r="F56" t="s">
-        <v>182</v>
+        <v>199</v>
       </c>
       <c r="G56" t="s">
         <v>34</v>
@@ -4899,7 +5293,7 @@
         <v>1</v>
       </c>
       <c r="J56" s="7" t="s">
-        <v>165</v>
+        <v>216</v>
       </c>
       <c r="K56">
         <v>1000</v>
@@ -4908,25 +5302,25 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>55</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>92</v>
+        <v>195</v>
       </c>
       <c r="C57" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D57" s="5">
         <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E57" t="s">
         <v>13</v>
       </c>
       <c r="F57" t="s">
-        <v>182</v>
+        <v>199</v>
       </c>
       <c r="G57" t="s">
         <v>151</v>
@@ -4938,7 +5332,7 @@
         <v>1</v>
       </c>
       <c r="J57" s="7" t="s">
-        <v>166</v>
+        <v>217</v>
       </c>
       <c r="K57">
         <v>1000</v>
@@ -4952,20 +5346,20 @@
         <v>56</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>93</v>
+        <v>196</v>
       </c>
       <c r="C58" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D58" s="5">
         <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E58" t="s">
         <v>11</v>
       </c>
       <c r="F58" t="s">
-        <v>183</v>
+        <v>200</v>
       </c>
       <c r="G58" t="s">
         <v>34</v>
@@ -4977,7 +5371,7 @@
         <v>1</v>
       </c>
       <c r="J58" s="7" t="s">
-        <v>149</v>
+        <v>218</v>
       </c>
       <c r="K58">
         <v>1000</v>
@@ -4986,25 +5380,25 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>57</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>94</v>
+        <v>209</v>
       </c>
       <c r="C59" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D59" s="5">
         <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E59" t="s">
         <v>14</v>
       </c>
       <c r="F59" t="s">
-        <v>183</v>
+        <v>200</v>
       </c>
       <c r="G59" t="s">
         <v>151</v>
@@ -5016,7 +5410,7 @@
         <v>1</v>
       </c>
       <c r="J59" s="7" t="s">
-        <v>150</v>
+        <v>219</v>
       </c>
       <c r="K59">
         <v>1000</v>
@@ -5030,20 +5424,20 @@
         <v>58</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>95</v>
+        <v>197</v>
       </c>
       <c r="C60" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D60" s="5">
         <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E60" t="s">
         <v>12</v>
       </c>
       <c r="F60" t="s">
-        <v>183</v>
+        <v>200</v>
       </c>
       <c r="G60" t="s">
         <v>34</v>
@@ -5055,7 +5449,7 @@
         <v>1</v>
       </c>
       <c r="J60" s="7" t="s">
-        <v>167</v>
+        <v>220</v>
       </c>
       <c r="K60">
         <v>1000</v>
@@ -5064,25 +5458,25 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>59</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>96</v>
+        <v>198</v>
       </c>
       <c r="C61" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D61" s="5">
         <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E61" t="s">
         <v>13</v>
       </c>
       <c r="F61" t="s">
-        <v>183</v>
+        <v>200</v>
       </c>
       <c r="G61" t="s">
         <v>151</v>
@@ -5094,7 +5488,7 @@
         <v>1</v>
       </c>
       <c r="J61" s="7" t="s">
-        <v>168</v>
+        <v>222</v>
       </c>
       <c r="K61">
         <v>1000</v>
@@ -5103,12 +5497,12 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>60</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C62" t="s">
         <v>27</v>
@@ -5121,7 +5515,7 @@
         <v>11</v>
       </c>
       <c r="F62" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G62" t="s">
         <v>34</v>
@@ -5133,7 +5527,7 @@
         <v>1</v>
       </c>
       <c r="J62" s="7" t="s">
-        <v>173</v>
+        <v>144</v>
       </c>
       <c r="K62">
         <v>1000</v>
@@ -5142,12 +5536,12 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>61</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>98</v>
+        <v>36</v>
       </c>
       <c r="C63" t="s">
         <v>27</v>
@@ -5160,19 +5554,19 @@
         <v>14</v>
       </c>
       <c r="F63" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G63" t="s">
-        <v>151</v>
+        <v>34</v>
       </c>
       <c r="H63" t="s">
-        <v>152</v>
+        <v>35</v>
       </c>
       <c r="I63" t="b">
         <v>1</v>
       </c>
       <c r="J63" s="7" t="s">
-        <v>174</v>
+        <v>145</v>
       </c>
       <c r="K63">
         <v>1000</v>
@@ -5181,12 +5575,12 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>62</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="C64" t="s">
         <v>27</v>
@@ -5199,7 +5593,7 @@
         <v>12</v>
       </c>
       <c r="F64" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G64" t="s">
         <v>34</v>
@@ -5211,7 +5605,7 @@
         <v>1</v>
       </c>
       <c r="J64" s="7" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="K64">
         <v>1000</v>
@@ -5220,12 +5614,12 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>63</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="C65" t="s">
         <v>27</v>
@@ -5238,19 +5632,19 @@
         <v>13</v>
       </c>
       <c r="F65" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G65" t="s">
-        <v>151</v>
+        <v>34</v>
       </c>
       <c r="H65" t="s">
-        <v>152</v>
+        <v>35</v>
       </c>
       <c r="I65" t="b">
         <v>1</v>
       </c>
       <c r="J65" s="7" t="s">
-        <v>176</v>
+        <v>147</v>
       </c>
       <c r="K65">
         <v>1000</v>
@@ -5259,12 +5653,12 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>64</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C66" t="s">
         <v>27</v>
@@ -5277,7 +5671,7 @@
         <v>11</v>
       </c>
       <c r="F66" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G66" t="s">
         <v>34</v>
@@ -5289,7 +5683,7 @@
         <v>1</v>
       </c>
       <c r="J66" s="7" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="K66">
         <v>1000</v>
@@ -5298,12 +5692,12 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>65</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="C67" t="s">
         <v>27</v>
@@ -5316,7 +5710,7 @@
         <v>14</v>
       </c>
       <c r="F67" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G67" t="s">
         <v>151</v>
@@ -5328,7 +5722,7 @@
         <v>1</v>
       </c>
       <c r="J67" s="7" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="K67">
         <v>1000</v>
@@ -5337,12 +5731,12 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>66</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="C68" t="s">
         <v>27</v>
@@ -5355,7 +5749,7 @@
         <v>12</v>
       </c>
       <c r="F68" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G68" t="s">
         <v>34</v>
@@ -5367,7 +5761,7 @@
         <v>1</v>
       </c>
       <c r="J68" s="7" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="K68">
         <v>1000</v>
@@ -5376,12 +5770,12 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>67</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C69" t="s">
         <v>27</v>
@@ -5394,7 +5788,7 @@
         <v>13</v>
       </c>
       <c r="F69" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G69" t="s">
         <v>151</v>
@@ -5406,7 +5800,7 @@
         <v>1</v>
       </c>
       <c r="J69" s="7" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="K69">
         <v>1000</v>
@@ -5415,12 +5809,12 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>68</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="C70" t="s">
         <v>27</v>
@@ -5433,7 +5827,7 @@
         <v>11</v>
       </c>
       <c r="F70" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G70" t="s">
         <v>34</v>
@@ -5445,7 +5839,7 @@
         <v>1</v>
       </c>
       <c r="J70" s="7" t="s">
-        <v>187</v>
+        <v>149</v>
       </c>
       <c r="K70">
         <v>1000</v>
@@ -5454,12 +5848,12 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>69</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="C71" t="s">
         <v>27</v>
@@ -5472,19 +5866,19 @@
         <v>14</v>
       </c>
       <c r="F71" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G71" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="H71" t="s">
-        <v>35</v>
+        <v>152</v>
       </c>
       <c r="I71" t="b">
         <v>1</v>
       </c>
       <c r="J71" s="7" t="s">
-        <v>187</v>
+        <v>150</v>
       </c>
       <c r="K71">
         <v>1000</v>
@@ -5493,12 +5887,12 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>70</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C72" t="s">
         <v>27</v>
@@ -5511,7 +5905,7 @@
         <v>12</v>
       </c>
       <c r="F72" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G72" t="s">
         <v>34</v>
@@ -5523,7 +5917,7 @@
         <v>1</v>
       </c>
       <c r="J72" s="7" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="K72">
         <v>1000</v>
@@ -5532,12 +5926,12 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>71</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C73" t="s">
         <v>27</v>
@@ -5550,7 +5944,7 @@
         <v>13</v>
       </c>
       <c r="F73" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G73" t="s">
         <v>151</v>
@@ -5562,12 +5956,480 @@
         <v>1</v>
       </c>
       <c r="J73" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="K73">
+        <v>1000</v>
+      </c>
+      <c r="L73">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>72</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C74" t="s">
+        <v>27</v>
+      </c>
+      <c r="D74" s="5">
+        <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="E74" t="s">
+        <v>11</v>
+      </c>
+      <c r="F74" t="s">
+        <v>184</v>
+      </c>
+      <c r="G74" t="s">
+        <v>34</v>
+      </c>
+      <c r="H74" t="s">
+        <v>35</v>
+      </c>
+      <c r="I74" t="b">
+        <v>1</v>
+      </c>
+      <c r="J74" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="K74">
+        <v>1000</v>
+      </c>
+      <c r="L74">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>73</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C75" t="s">
+        <v>27</v>
+      </c>
+      <c r="D75" s="5">
+        <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="E75" t="s">
+        <v>14</v>
+      </c>
+      <c r="F75" t="s">
+        <v>184</v>
+      </c>
+      <c r="G75" t="s">
+        <v>151</v>
+      </c>
+      <c r="H75" t="s">
+        <v>152</v>
+      </c>
+      <c r="I75" t="b">
+        <v>1</v>
+      </c>
+      <c r="J75" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="K75">
+        <v>1000</v>
+      </c>
+      <c r="L75">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>74</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C76" t="s">
+        <v>27</v>
+      </c>
+      <c r="D76" s="5">
+        <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="E76" t="s">
+        <v>12</v>
+      </c>
+      <c r="F76" t="s">
+        <v>184</v>
+      </c>
+      <c r="G76" t="s">
+        <v>34</v>
+      </c>
+      <c r="H76" t="s">
+        <v>35</v>
+      </c>
+      <c r="I76" t="b">
+        <v>1</v>
+      </c>
+      <c r="J76" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="K76">
+        <v>1000</v>
+      </c>
+      <c r="L76">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>75</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C77" t="s">
+        <v>27</v>
+      </c>
+      <c r="D77" s="5">
+        <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="E77" t="s">
+        <v>13</v>
+      </c>
+      <c r="F77" t="s">
+        <v>184</v>
+      </c>
+      <c r="G77" t="s">
+        <v>151</v>
+      </c>
+      <c r="H77" t="s">
+        <v>152</v>
+      </c>
+      <c r="I77" t="b">
+        <v>1</v>
+      </c>
+      <c r="J77" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="K77">
+        <v>1000</v>
+      </c>
+      <c r="L77">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>76</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C78" t="s">
+        <v>27</v>
+      </c>
+      <c r="D78" s="5">
+        <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="E78" t="s">
+        <v>11</v>
+      </c>
+      <c r="F78" t="s">
+        <v>185</v>
+      </c>
+      <c r="G78" t="s">
+        <v>34</v>
+      </c>
+      <c r="H78" t="s">
+        <v>35</v>
+      </c>
+      <c r="I78" t="b">
+        <v>1</v>
+      </c>
+      <c r="J78" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="K78">
+        <v>1000</v>
+      </c>
+      <c r="L78">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>77</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C79" t="s">
+        <v>27</v>
+      </c>
+      <c r="D79" s="5">
+        <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="E79" t="s">
+        <v>14</v>
+      </c>
+      <c r="F79" t="s">
+        <v>185</v>
+      </c>
+      <c r="G79" t="s">
+        <v>151</v>
+      </c>
+      <c r="H79" t="s">
+        <v>152</v>
+      </c>
+      <c r="I79" t="b">
+        <v>1</v>
+      </c>
+      <c r="J79" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="K79">
+        <v>1000</v>
+      </c>
+      <c r="L79">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>78</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C80" t="s">
+        <v>27</v>
+      </c>
+      <c r="D80" s="5">
+        <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="E80" t="s">
+        <v>12</v>
+      </c>
+      <c r="F80" t="s">
+        <v>185</v>
+      </c>
+      <c r="G80" t="s">
+        <v>34</v>
+      </c>
+      <c r="H80" t="s">
+        <v>35</v>
+      </c>
+      <c r="I80" t="b">
+        <v>1</v>
+      </c>
+      <c r="J80" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="K80">
+        <v>1000</v>
+      </c>
+      <c r="L80">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>79</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C81" t="s">
+        <v>27</v>
+      </c>
+      <c r="D81" s="5">
+        <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="E81" t="s">
+        <v>13</v>
+      </c>
+      <c r="F81" t="s">
+        <v>185</v>
+      </c>
+      <c r="G81" t="s">
+        <v>151</v>
+      </c>
+      <c r="H81" t="s">
+        <v>152</v>
+      </c>
+      <c r="I81" t="b">
+        <v>1</v>
+      </c>
+      <c r="J81" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="K81">
+        <v>1000</v>
+      </c>
+      <c r="L81">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>80</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C82" t="s">
+        <v>27</v>
+      </c>
+      <c r="D82" s="5">
+        <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="E82" t="s">
+        <v>11</v>
+      </c>
+      <c r="F82" t="s">
+        <v>186</v>
+      </c>
+      <c r="G82" t="s">
+        <v>34</v>
+      </c>
+      <c r="H82" t="s">
+        <v>35</v>
+      </c>
+      <c r="I82" t="b">
+        <v>1</v>
+      </c>
+      <c r="J82" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="K82">
+        <v>1000</v>
+      </c>
+      <c r="L82">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>81</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="C83" t="s">
+        <v>27</v>
+      </c>
+      <c r="D83" s="5">
+        <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="E83" t="s">
+        <v>14</v>
+      </c>
+      <c r="F83" t="s">
+        <v>186</v>
+      </c>
+      <c r="G83" t="s">
+        <v>151</v>
+      </c>
+      <c r="H83" t="s">
+        <v>152</v>
+      </c>
+      <c r="I83" t="b">
+        <v>1</v>
+      </c>
+      <c r="J83" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="K83">
+        <v>1000</v>
+      </c>
+      <c r="L83">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>82</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C84" t="s">
+        <v>27</v>
+      </c>
+      <c r="D84" s="5">
+        <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="E84" t="s">
+        <v>12</v>
+      </c>
+      <c r="F84" t="s">
+        <v>186</v>
+      </c>
+      <c r="G84" t="s">
+        <v>34</v>
+      </c>
+      <c r="H84" t="s">
+        <v>35</v>
+      </c>
+      <c r="I84" t="b">
+        <v>1</v>
+      </c>
+      <c r="J84" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="K84">
+        <v>1000</v>
+      </c>
+      <c r="L84">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>83</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C85" t="s">
+        <v>27</v>
+      </c>
+      <c r="D85" s="5">
+        <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="E85" t="s">
+        <v>13</v>
+      </c>
+      <c r="F85" t="s">
+        <v>186</v>
+      </c>
+      <c r="G85" t="s">
+        <v>151</v>
+      </c>
+      <c r="H85" t="s">
+        <v>152</v>
+      </c>
+      <c r="I85" t="b">
+        <v>1</v>
+      </c>
+      <c r="J85" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="K73">
-        <v>1000</v>
-      </c>
-      <c r="L73">
+      <c r="K85">
+        <v>1000</v>
+      </c>
+      <c r="L85">
         <v>1000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added model weights to experiment
</commit_message>
<xml_diff>
--- a/model_config.xlsx
+++ b/model_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asafsilman/Desktop/GENG5511/GalaxyEnvironmentAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2FAF1B-AF3F-034E-AD12-98392051772F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A013F8-7B4F-6B4C-8168-48A96C3AB5CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" activeTab="1" xr2:uid="{DA573336-42C9-534D-A3C9-C8C047CC3E2B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" xr2:uid="{DA573336-42C9-534D-A3C9-C8C047CC3E2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="227">
   <si>
     <t>modelName</t>
   </si>
@@ -713,6 +713,9 @@
   </si>
   <si>
     <t>7f60221c52e74c29630b1a8d206fa4d0d1b7af9b757a333a8fb91f3049d2e908</t>
+  </si>
+  <si>
+    <t>dataSet_m9</t>
   </si>
 </sst>
 </file>
@@ -779,9 +782,16 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="22">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -802,6 +812,49 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -861,6 +914,26 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -875,26 +948,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BFE53D84-975D-9E44-A5C0-0D53C58F4B56}" name="Table3" displayName="Table3" ref="A1:T31" totalsRowShown="0">
-  <autoFilter ref="A1:T31" xr:uid="{CC0FBD37-8587-624E-8633-B9595665FD07}"/>
-  <tableColumns count="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BFE53D84-975D-9E44-A5C0-0D53C58F4B56}" name="Table3" displayName="Table3" ref="A1:U31" totalsRowShown="0">
+  <autoFilter ref="A1:U31" xr:uid="{CC0FBD37-8587-624E-8633-B9595665FD07}"/>
+  <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{703C2328-6727-224A-92DA-FB21A475BF4C}" name="modelId"/>
     <tableColumn id="5" xr3:uid="{091AFF89-BAE7-674D-85D8-5FA5B7DAF36C}" name="modelAltName"/>
-    <tableColumn id="6" xr3:uid="{9243668A-FEFC-2A44-85FD-E9850DCD3F13}" name="modelName" dataDxfId="14">
+    <tableColumn id="6" xr3:uid="{9243668A-FEFC-2A44-85FD-E9850DCD3F13}" name="modelName" dataDxfId="19">
       <calculatedColumnFormula>_xlfn.CONCAT(Table3[[#This Row],[numChannels]],"_channel_",Table3[[#This Row],[modelType]],"_", Table3[[#This Row],[_modelNameString]], "_", Table3[[#This Row],[_modelDataString]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{E6DF2D56-96C3-AF43-9D19-75691A5B5160}" name="_modelNameString" dataDxfId="13">
+    <tableColumn id="20" xr3:uid="{E6DF2D56-96C3-AF43-9D19-75691A5B5160}" name="_modelNameString" dataDxfId="18">
       <calculatedColumnFormula>_xlfn.CONCAT(Table3[[#This Row],[channel1]], IF(Table3[[#This Row],[channel2]]&lt;&gt;"", _xlfn.CONCAT("_",Table3[[#This Row],[channel2]], IF(Table3[[#This Row],[channel3]]&lt;&gt;"", _xlfn.CONCAT("_", Table3[[#This Row],[channel3]]), ""), ""), ""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{25197AF6-7EB6-9344-B947-E907FA36108D}" name="_modelDataString" dataDxfId="0">
-      <calculatedColumnFormula>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</calculatedColumnFormula>
+    <tableColumn id="21" xr3:uid="{25197AF6-7EB6-9344-B947-E907FA36108D}" name="_modelDataString" dataDxfId="7">
+      <calculatedColumnFormula>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{A721B211-0E17-F640-A300-BE3E08E93596}" name="modelType" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{4347DEF6-17C0-3F43-802E-86E8674A6FB3}" name="numChannels" dataDxfId="11"/>
-    <tableColumn id="13" xr3:uid="{3B4B9348-11DD-394A-9D6A-D4850CC40194}" name="channel1" dataDxfId="10"/>
-    <tableColumn id="14" xr3:uid="{B526A24F-2ECC-0442-9CEB-DA811FF165E2}" name="channel2" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{0052B57A-E822-0B40-8C1E-8D026B8A57CC}" name="channel3" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{7E2B00ED-F5EB-4648-9E53-8AB3EC8A396B}" name="channel4" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{A721B211-0E17-F640-A300-BE3E08E93596}" name="modelType" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{4347DEF6-17C0-3F43-802E-86E8674A6FB3}" name="numChannels" dataDxfId="16"/>
+    <tableColumn id="13" xr3:uid="{3B4B9348-11DD-394A-9D6A-D4850CC40194}" name="channel1" dataDxfId="15"/>
+    <tableColumn id="14" xr3:uid="{B526A24F-2ECC-0442-9CEB-DA811FF165E2}" name="channel2" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{0052B57A-E822-0B40-8C1E-8D026B8A57CC}" name="channel3" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{7E2B00ED-F5EB-4648-9E53-8AB3EC8A396B}" name="channel4" dataDxfId="12"/>
     <tableColumn id="9" xr3:uid="{712BD42A-DEBB-2545-A3FE-8F98C541BB5F}" name="dataSet_m1"/>
     <tableColumn id="10" xr3:uid="{1C7EA2DE-42E0-4949-B9B8-64BD2A71AC95}" name="dataSet_m2"/>
     <tableColumn id="11" xr3:uid="{82D55CF4-DECF-6844-ABEC-7EC6D1BC5DA6}" name="dataSet_m3"/>
@@ -904,19 +977,20 @@
     <tableColumn id="17" xr3:uid="{EAB20F55-7FD9-224C-A3DB-181D5CB1A345}" name="dataSet_m6"/>
     <tableColumn id="12" xr3:uid="{D0D85B70-32C3-1546-9D25-48EF6AA9A2E2}" name="dataSet_m7"/>
     <tableColumn id="18" xr3:uid="{36F61E23-086F-BD45-812C-CAA7CE0D0D34}" name="dataSet_m8"/>
+    <tableColumn id="19" xr3:uid="{21B6B59B-D73B-4242-97CE-4E3DF0B45BA0}" name="dataSet_m9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BBA15079-BA5C-4347-AB18-D63DE85A40E7}" name="Table1" displayName="Table1" ref="A1:L85" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BBA15079-BA5C-4347-AB18-D63DE85A40E7}" name="Table1" displayName="Table1" ref="A1:L85" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="A1:L85" xr:uid="{1608FF67-3914-5949-96DC-606C50EA2E4D}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{AE589D12-F9F2-7E46-B3F1-011FE87BB9E7}" name="dataId"/>
-    <tableColumn id="2" xr3:uid="{86A820C4-44CA-F647-A338-3C42F8D54CAF}" name="dataFile" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{86A820C4-44CA-F647-A338-3C42F8D54CAF}" name="dataFile" dataDxfId="10"/>
     <tableColumn id="3" xr3:uid="{8CB7439C-328A-4840-8650-53C68739CB52}" name="dataLabel"/>
-    <tableColumn id="6" xr3:uid="{20416ED2-C6CE-DB4D-BCD0-4920296FFAB5}" name="dataLabelValue" dataDxfId="4">
+    <tableColumn id="6" xr3:uid="{20416ED2-C6CE-DB4D-BCD0-4920296FFAB5}" name="dataLabelValue" dataDxfId="9">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{ECFC63C3-8324-5B40-8261-525DCDBB1D77}" name="dataSimType"/>
@@ -924,7 +998,7 @@
     <tableColumn id="7" xr3:uid="{A34CD7B0-6947-5A42-AD6C-DDCF954D6599}" name="imageFileName"/>
     <tableColumn id="8" xr3:uid="{4E77CFD9-0959-1946-94BB-C03C9823FFCF}" name="labelFileName"/>
     <tableColumn id="10" xr3:uid="{B5582984-20BB-B04C-ACD1-B32B5C014342}" name="fileAvailable"/>
-    <tableColumn id="9" xr3:uid="{8E67EC6E-99AC-7043-8F51-B1C73A2D564B}" name="fileHash" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{8E67EC6E-99AC-7043-8F51-B1C73A2D564B}" name="fileHash" dataDxfId="8"/>
     <tableColumn id="11" xr3:uid="{38F53538-5DB0-E34C-B916-D0BD7FD2CC71}" name="imageFileNumRows"/>
     <tableColumn id="12" xr3:uid="{E263E244-E409-B344-BD21-61A040BA1A1C}" name="labelFileNumRows"/>
   </tableColumns>
@@ -1240,10 +1314,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F969F3E7-5EBB-B140-87B5-F57642023AAB}">
-  <dimension ref="A1:T31"/>
+  <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7:U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1263,7 +1337,7 @@
     <col min="17" max="18" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1324,8 +1398,11 @@
       <c r="T1" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1338,7 +1415,7 @@
         <v>gas_density</v>
       </c>
       <c r="E2" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -1380,8 +1457,11 @@
       <c r="T2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1394,7 +1474,7 @@
         <v>gas_kinematics</v>
       </c>
       <c r="E3" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1436,8 +1516,11 @@
       <c r="T3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1450,7 +1533,7 @@
         <v>star_density</v>
       </c>
       <c r="E4" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -1492,8 +1575,11 @@
       <c r="T4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1506,7 +1592,7 @@
         <v>star_kinematics</v>
       </c>
       <c r="E5" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -1548,8 +1634,11 @@
       <c r="T5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1562,7 +1651,7 @@
         <v>gas_density_star_density</v>
       </c>
       <c r="E6" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -1606,8 +1695,11 @@
       <c r="T6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1620,7 +1712,7 @@
         <v>gas_density_star_kinematics</v>
       </c>
       <c r="E7" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -1664,8 +1756,11 @@
       <c r="T7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1678,7 +1773,7 @@
         <v>gas_kinematics_star_density</v>
       </c>
       <c r="E8" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -1722,8 +1817,11 @@
       <c r="T8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1736,7 +1834,7 @@
         <v>gas_kinematics_star_kinematics</v>
       </c>
       <c r="E9" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -1780,8 +1878,11 @@
       <c r="T9" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1794,7 +1895,7 @@
         <v>gas_density_gas_kinematics</v>
       </c>
       <c r="E10" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -1838,8 +1939,11 @@
       <c r="T10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1852,7 +1956,7 @@
         <v>star_density_star_kinematics</v>
       </c>
       <c r="E11" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F11" s="1" t="s">
@@ -1896,8 +2000,11 @@
       <c r="T11" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1910,7 +2017,7 @@
         <v>gas_density_gas_kinematics_star_density</v>
       </c>
       <c r="E12" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -1956,8 +2063,11 @@
       <c r="T12" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1970,7 +2080,7 @@
         <v>gas_density_gas_kinematics_star_density</v>
       </c>
       <c r="E13" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F13" s="1" t="s">
@@ -2016,8 +2126,11 @@
       <c r="T13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2030,7 +2143,7 @@
         <v>gas_density_star_density_star_kinematics</v>
       </c>
       <c r="E14" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F14" s="1" t="s">
@@ -2076,8 +2189,11 @@
       <c r="T14" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2090,7 +2206,7 @@
         <v>gas_kinematics_star_density_star_kinematics</v>
       </c>
       <c r="E15" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F15" s="1" t="s">
@@ -2136,8 +2252,11 @@
       <c r="T15" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2153,7 +2272,7 @@
         <v>gas_density_gas_kinematics_star_density</v>
       </c>
       <c r="E16" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F16" s="1" t="s">
@@ -2201,8 +2320,11 @@
       <c r="T16" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2215,7 +2337,7 @@
         <v>gas_density</v>
       </c>
       <c r="E17" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F17" s="1" t="s">
@@ -2257,8 +2379,11 @@
       <c r="T17" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2271,7 +2396,7 @@
         <v>gas_kinematics</v>
       </c>
       <c r="E18" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F18" s="1" t="s">
@@ -2313,8 +2438,11 @@
       <c r="T18" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2327,7 +2455,7 @@
         <v>star_density</v>
       </c>
       <c r="E19" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F19" s="1" t="s">
@@ -2369,8 +2497,11 @@
       <c r="T19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2383,7 +2514,7 @@
         <v>star_kinematics</v>
       </c>
       <c r="E20" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F20" s="1" t="s">
@@ -2425,8 +2556,11 @@
       <c r="T20" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2439,7 +2573,7 @@
         <v>gas_density_star_density</v>
       </c>
       <c r="E21" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F21" s="1" t="s">
@@ -2483,8 +2617,11 @@
       <c r="T21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2497,7 +2634,7 @@
         <v>gas_density_star_kinematics</v>
       </c>
       <c r="E22" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F22" s="1" t="s">
@@ -2541,8 +2678,11 @@
       <c r="T22" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2555,7 +2695,7 @@
         <v>gas_kinematics_star_density</v>
       </c>
       <c r="E23" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F23" s="1" t="s">
@@ -2599,8 +2739,11 @@
       <c r="T23" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2613,7 +2756,7 @@
         <v>gas_kinematics_star_kinematics</v>
       </c>
       <c r="E24" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F24" s="1" t="s">
@@ -2657,8 +2800,11 @@
       <c r="T24" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2671,7 +2817,7 @@
         <v>gas_density_gas_kinematics</v>
       </c>
       <c r="E25" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F25" s="1" t="s">
@@ -2715,8 +2861,11 @@
       <c r="T25" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2729,7 +2878,7 @@
         <v>star_density_star_kinematics</v>
       </c>
       <c r="E26" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F26" s="1" t="s">
@@ -2773,8 +2922,11 @@
       <c r="T26" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2787,7 +2939,7 @@
         <v>gas_density_gas_kinematics_star_density</v>
       </c>
       <c r="E27" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F27" s="1" t="s">
@@ -2833,8 +2985,11 @@
       <c r="T27" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2847,7 +3002,7 @@
         <v>gas_density_gas_kinematics_star_density</v>
       </c>
       <c r="E28" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F28" s="1" t="s">
@@ -2893,8 +3048,11 @@
       <c r="T28" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2907,7 +3065,7 @@
         <v>gas_density_star_density_star_kinematics</v>
       </c>
       <c r="E29" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F29" s="1" t="s">
@@ -2953,8 +3111,11 @@
       <c r="T29" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2967,7 +3128,7 @@
         <v>gas_kinematics_star_density_star_kinematics</v>
       </c>
       <c r="E30" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F30" s="1" t="s">
@@ -3013,8 +3174,11 @@
       <c r="T30" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -3030,7 +3194,7 @@
         <v>gas_density_gas_kinematics_star_density</v>
       </c>
       <c r="E31" t="str">
-        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")</f>
+        <f>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</f>
         <v>m1m2m3</v>
       </c>
       <c r="F31" s="1" t="s">
@@ -3078,16 +3242,24 @@
       <c r="T31" t="b">
         <v>0</v>
       </c>
+      <c r="U31" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="L2:N31 P2:T31">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+  <conditionalFormatting sqref="L2:N31 P2:U6 P8:U31">
+    <cfRule type="cellIs" dxfId="21" priority="9" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O2:O31">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="O2:O6 O8:O31">
+    <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O7:U7">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3102,7 +3274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A15A60-C633-ED48-8690-686D42EE8C24}">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="L58" sqref="L58"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added rps m10 data to repo
</commit_message>
<xml_diff>
--- a/model_config.xlsx
+++ b/model_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asafsilman/Desktop/GENG5511/GalaxyEnvironmentAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A013F8-7B4F-6B4C-8168-48A96C3AB5CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448BAC6A-7FBA-0D46-A882-40BADBA3B350}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" xr2:uid="{DA573336-42C9-534D-A3C9-C8C047CC3E2B}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="16100" activeTab="1" xr2:uid="{DA573336-42C9-534D-A3C9-C8C047CC3E2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="232">
   <si>
     <t>modelName</t>
   </si>
@@ -634,12 +634,6 @@
     <t>A.rs.m9v.dir.tar.gz</t>
   </si>
   <si>
-    <t>m8</t>
-  </si>
-  <si>
-    <t>m9</t>
-  </si>
-  <si>
     <t>m4a</t>
   </si>
   <si>
@@ -716,6 +710,27 @@
   </si>
   <si>
     <t>dataSet_m9</t>
+  </si>
+  <si>
+    <t>m5a</t>
+  </si>
+  <si>
+    <t>m6a</t>
+  </si>
+  <si>
+    <t>A.r.m10.dir.tar.gz</t>
+  </si>
+  <si>
+    <t>A.r.m10v.dir.tar.gz</t>
+  </si>
+  <si>
+    <t>m7</t>
+  </si>
+  <si>
+    <t>a911a60cbb77134f3e10d78d562666626f42c6a384bf279d805f28d385f62d03</t>
+  </si>
+  <si>
+    <t>be25cf43a21588ab87eabed9ae24a022797cc02397ee4edc8762f5a86fd2e786</t>
   </si>
 </sst>
 </file>
@@ -782,7 +797,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="16">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -812,49 +827,6 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -915,24 +887,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -953,21 +908,21 @@
   <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{703C2328-6727-224A-92DA-FB21A475BF4C}" name="modelId"/>
     <tableColumn id="5" xr3:uid="{091AFF89-BAE7-674D-85D8-5FA5B7DAF36C}" name="modelAltName"/>
-    <tableColumn id="6" xr3:uid="{9243668A-FEFC-2A44-85FD-E9850DCD3F13}" name="modelName" dataDxfId="19">
+    <tableColumn id="6" xr3:uid="{9243668A-FEFC-2A44-85FD-E9850DCD3F13}" name="modelName" dataDxfId="15">
       <calculatedColumnFormula>_xlfn.CONCAT(Table3[[#This Row],[numChannels]],"_channel_",Table3[[#This Row],[modelType]],"_", Table3[[#This Row],[_modelNameString]], "_", Table3[[#This Row],[_modelDataString]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{E6DF2D56-96C3-AF43-9D19-75691A5B5160}" name="_modelNameString" dataDxfId="18">
+    <tableColumn id="20" xr3:uid="{E6DF2D56-96C3-AF43-9D19-75691A5B5160}" name="_modelNameString" dataDxfId="14">
       <calculatedColumnFormula>_xlfn.CONCAT(Table3[[#This Row],[channel1]], IF(Table3[[#This Row],[channel2]]&lt;&gt;"", _xlfn.CONCAT("_",Table3[[#This Row],[channel2]], IF(Table3[[#This Row],[channel3]]&lt;&gt;"", _xlfn.CONCAT("_", Table3[[#This Row],[channel3]]), ""), ""), ""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{25197AF6-7EB6-9344-B947-E907FA36108D}" name="_modelDataString" dataDxfId="7">
+    <tableColumn id="21" xr3:uid="{25197AF6-7EB6-9344-B947-E907FA36108D}" name="_modelDataString" dataDxfId="13">
       <calculatedColumnFormula>IF(Table3[[#This Row],[dataSet_m1]], "m1", "")&amp;IF(Table3[[#This Row],[dataSet_m2]], "m2", "")&amp;IF(Table3[[#This Row],[dataSet_m3]], "m3", "")&amp;IF(Table3[[#This Row],[dataSet_m4]], "m4", "")&amp;IF(Table3[[#This Row],[dataSet_m4a]], "m4a", "")&amp;IF(Table3[[#This Row],[dataSet_m5]], "m5", "")&amp;IF(Table3[[#This Row],[dataSet_m6]], "m6", "")&amp;IF(Table3[[#This Row],[dataSet_m7]], "m7", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m8", "")&amp;IF(Table3[[#This Row],[dataSet_m8]], "m9", "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{A721B211-0E17-F640-A300-BE3E08E93596}" name="modelType" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{4347DEF6-17C0-3F43-802E-86E8674A6FB3}" name="numChannels" dataDxfId="16"/>
-    <tableColumn id="13" xr3:uid="{3B4B9348-11DD-394A-9D6A-D4850CC40194}" name="channel1" dataDxfId="15"/>
-    <tableColumn id="14" xr3:uid="{B526A24F-2ECC-0442-9CEB-DA811FF165E2}" name="channel2" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{0052B57A-E822-0B40-8C1E-8D026B8A57CC}" name="channel3" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{7E2B00ED-F5EB-4648-9E53-8AB3EC8A396B}" name="channel4" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{A721B211-0E17-F640-A300-BE3E08E93596}" name="modelType" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{4347DEF6-17C0-3F43-802E-86E8674A6FB3}" name="numChannels" dataDxfId="11"/>
+    <tableColumn id="13" xr3:uid="{3B4B9348-11DD-394A-9D6A-D4850CC40194}" name="channel1" dataDxfId="10"/>
+    <tableColumn id="14" xr3:uid="{B526A24F-2ECC-0442-9CEB-DA811FF165E2}" name="channel2" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{0052B57A-E822-0B40-8C1E-8D026B8A57CC}" name="channel3" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{7E2B00ED-F5EB-4648-9E53-8AB3EC8A396B}" name="channel4" dataDxfId="7"/>
     <tableColumn id="9" xr3:uid="{712BD42A-DEBB-2545-A3FE-8F98C541BB5F}" name="dataSet_m1"/>
     <tableColumn id="10" xr3:uid="{1C7EA2DE-42E0-4949-B9B8-64BD2A71AC95}" name="dataSet_m2"/>
     <tableColumn id="11" xr3:uid="{82D55CF4-DECF-6844-ABEC-7EC6D1BC5DA6}" name="dataSet_m3"/>
@@ -984,13 +939,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BBA15079-BA5C-4347-AB18-D63DE85A40E7}" name="Table1" displayName="Table1" ref="A1:L85" totalsRowShown="0" headerRowDxfId="11">
-  <autoFilter ref="A1:L85" xr:uid="{1608FF67-3914-5949-96DC-606C50EA2E4D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BBA15079-BA5C-4347-AB18-D63DE85A40E7}" name="Table1" displayName="Table1" ref="A1:L87" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:L87" xr:uid="{1608FF67-3914-5949-96DC-606C50EA2E4D}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{AE589D12-F9F2-7E46-B3F1-011FE87BB9E7}" name="dataId"/>
-    <tableColumn id="2" xr3:uid="{86A820C4-44CA-F647-A338-3C42F8D54CAF}" name="dataFile" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{86A820C4-44CA-F647-A338-3C42F8D54CAF}" name="dataFile" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{8CB7439C-328A-4840-8650-53C68739CB52}" name="dataLabel"/>
-    <tableColumn id="6" xr3:uid="{20416ED2-C6CE-DB4D-BCD0-4920296FFAB5}" name="dataLabelValue" dataDxfId="9">
+    <tableColumn id="6" xr3:uid="{20416ED2-C6CE-DB4D-BCD0-4920296FFAB5}" name="dataLabelValue" dataDxfId="4">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{ECFC63C3-8324-5B40-8261-525DCDBB1D77}" name="dataSimType"/>
@@ -998,7 +953,7 @@
     <tableColumn id="7" xr3:uid="{A34CD7B0-6947-5A42-AD6C-DDCF954D6599}" name="imageFileName"/>
     <tableColumn id="8" xr3:uid="{4E77CFD9-0959-1946-94BB-C03C9823FFCF}" name="labelFileName"/>
     <tableColumn id="10" xr3:uid="{B5582984-20BB-B04C-ACD1-B32B5C014342}" name="fileAvailable"/>
-    <tableColumn id="9" xr3:uid="{8E67EC6E-99AC-7043-8F51-B1C73A2D564B}" name="fileHash" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{8E67EC6E-99AC-7043-8F51-B1C73A2D564B}" name="fileHash" dataDxfId="3"/>
     <tableColumn id="11" xr3:uid="{38F53538-5DB0-E34C-B916-D0BD7FD2CC71}" name="imageFileNumRows"/>
     <tableColumn id="12" xr3:uid="{E263E244-E409-B344-BD21-61A040BA1A1C}" name="labelFileNumRows"/>
   </tableColumns>
@@ -1316,7 +1271,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F969F3E7-5EBB-B140-87B5-F57642023AAB}">
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O7" sqref="O7:U7"/>
     </sheetView>
   </sheetViews>
@@ -1384,7 +1339,7 @@
         <v>8</v>
       </c>
       <c r="P1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="Q1" t="s">
         <v>9</v>
@@ -1393,13 +1348,13 @@
         <v>10</v>
       </c>
       <c r="S1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="T1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="U1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
@@ -3249,12 +3204,12 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="L2:N31 P2:U6 P8:U31">
-    <cfRule type="cellIs" dxfId="21" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="9" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O6 O8:O31">
-    <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3272,10 +3227,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A15A60-C633-ED48-8690-686D42EE8C24}">
-  <dimension ref="A1:L85"/>
+  <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L58" sqref="L58"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K62" sqref="K62:L62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3284,7 +3239,8 @@
     <col min="4" max="4" width="16.33203125" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" customWidth="1"/>
     <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="77.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.5" bestFit="1" customWidth="1"/>
@@ -4153,7 +4109,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C23" t="s">
         <v>25</v>
@@ -4178,7 +4134,7 @@
         <v>1</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="K23">
         <v>1000</v>
@@ -4751,7 +4707,7 @@
         <v>11</v>
       </c>
       <c r="F38" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G38" t="s">
         <v>34</v>
@@ -4790,7 +4746,7 @@
         <v>14</v>
       </c>
       <c r="F39" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G39" t="s">
         <v>151</v>
@@ -4829,7 +4785,7 @@
         <v>12</v>
       </c>
       <c r="F40" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G40" t="s">
         <v>34</v>
@@ -4868,7 +4824,7 @@
         <v>13</v>
       </c>
       <c r="F41" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G41" t="s">
         <v>151</v>
@@ -4907,7 +4863,7 @@
         <v>11</v>
       </c>
       <c r="F42" t="s">
-        <v>185</v>
+        <v>225</v>
       </c>
       <c r="G42" t="s">
         <v>34</v>
@@ -4946,7 +4902,7 @@
         <v>14</v>
       </c>
       <c r="F43" t="s">
-        <v>185</v>
+        <v>225</v>
       </c>
       <c r="G43" t="s">
         <v>151</v>
@@ -4985,7 +4941,7 @@
         <v>12</v>
       </c>
       <c r="F44" t="s">
-        <v>185</v>
+        <v>225</v>
       </c>
       <c r="G44" t="s">
         <v>34</v>
@@ -5024,7 +4980,7 @@
         <v>13</v>
       </c>
       <c r="F45" t="s">
-        <v>185</v>
+        <v>225</v>
       </c>
       <c r="G45" t="s">
         <v>151</v>
@@ -5063,7 +5019,7 @@
         <v>11</v>
       </c>
       <c r="F46" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="G46" t="s">
         <v>34</v>
@@ -5089,7 +5045,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C47" t="s">
         <v>26</v>
@@ -5102,7 +5058,7 @@
         <v>14</v>
       </c>
       <c r="F47" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="G47" t="s">
         <v>151</v>
@@ -5114,7 +5070,7 @@
         <v>1</v>
       </c>
       <c r="J47" s="7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K47">
         <v>500</v>
@@ -5141,7 +5097,7 @@
         <v>12</v>
       </c>
       <c r="F48" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="G48" t="s">
         <v>34</v>
@@ -5180,7 +5136,7 @@
         <v>13</v>
       </c>
       <c r="F49" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="G49" t="s">
         <v>151</v>
@@ -5231,7 +5187,7 @@
         <v>1</v>
       </c>
       <c r="J50" s="7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="K50">
         <v>1000</v>
@@ -5245,7 +5201,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C51" t="s">
         <v>26</v>
@@ -5270,7 +5226,7 @@
         <v>1</v>
       </c>
       <c r="J51" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K51">
         <v>1000</v>
@@ -5309,7 +5265,7 @@
         <v>1</v>
       </c>
       <c r="J52" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="K52">
         <v>1000</v>
@@ -5348,7 +5304,7 @@
         <v>1</v>
       </c>
       <c r="J53" s="7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K53">
         <v>1000</v>
@@ -5375,7 +5331,7 @@
         <v>11</v>
       </c>
       <c r="F54" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="G54" t="s">
         <v>34</v>
@@ -5387,7 +5343,7 @@
         <v>1</v>
       </c>
       <c r="J54" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K54">
         <v>1000</v>
@@ -5401,7 +5357,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C55" t="s">
         <v>26</v>
@@ -5414,7 +5370,7 @@
         <v>14</v>
       </c>
       <c r="F55" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="G55" t="s">
         <v>151</v>
@@ -5426,7 +5382,7 @@
         <v>1</v>
       </c>
       <c r="J55" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K55">
         <v>1000</v>
@@ -5453,7 +5409,7 @@
         <v>12</v>
       </c>
       <c r="F56" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="G56" t="s">
         <v>34</v>
@@ -5465,7 +5421,7 @@
         <v>1</v>
       </c>
       <c r="J56" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="K56">
         <v>1000</v>
@@ -5492,7 +5448,7 @@
         <v>13</v>
       </c>
       <c r="F57" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="G57" t="s">
         <v>151</v>
@@ -5504,7 +5460,7 @@
         <v>1</v>
       </c>
       <c r="J57" s="7" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="K57">
         <v>1000</v>
@@ -5531,7 +5487,7 @@
         <v>11</v>
       </c>
       <c r="F58" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="G58" t="s">
         <v>34</v>
@@ -5543,7 +5499,7 @@
         <v>1</v>
       </c>
       <c r="J58" s="7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="K58">
         <v>1000</v>
@@ -5557,7 +5513,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C59" t="s">
         <v>26</v>
@@ -5570,7 +5526,7 @@
         <v>14</v>
       </c>
       <c r="F59" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="G59" t="s">
         <v>151</v>
@@ -5582,7 +5538,7 @@
         <v>1</v>
       </c>
       <c r="J59" s="7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="K59">
         <v>1000</v>
@@ -5609,7 +5565,7 @@
         <v>12</v>
       </c>
       <c r="F60" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="G60" t="s">
         <v>34</v>
@@ -5621,7 +5577,7 @@
         <v>1</v>
       </c>
       <c r="J60" s="7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="K60">
         <v>1000</v>
@@ -5648,7 +5604,7 @@
         <v>13</v>
       </c>
       <c r="F61" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="G61" t="s">
         <v>151</v>
@@ -5660,7 +5616,7 @@
         <v>1</v>
       </c>
       <c r="J61" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="K61">
         <v>1000</v>
@@ -5674,20 +5630,20 @@
         <v>60</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>86</v>
+        <v>227</v>
       </c>
       <c r="C62" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D62" s="5">
         <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E62" t="s">
         <v>11</v>
       </c>
       <c r="F62" t="s">
-        <v>181</v>
+        <v>229</v>
       </c>
       <c r="G62" t="s">
         <v>34</v>
@@ -5699,13 +5655,13 @@
         <v>1</v>
       </c>
       <c r="J62" s="7" t="s">
-        <v>144</v>
+        <v>231</v>
       </c>
       <c r="K62">
-        <v>1000</v>
+        <v>30000</v>
       </c>
       <c r="L62">
-        <v>1000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
@@ -5713,38 +5669,38 @@
         <v>61</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>36</v>
+        <v>228</v>
       </c>
       <c r="C63" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D63" s="5">
         <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E63" t="s">
         <v>14</v>
       </c>
       <c r="F63" t="s">
-        <v>181</v>
+        <v>229</v>
       </c>
       <c r="G63" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="H63" t="s">
-        <v>35</v>
+        <v>152</v>
       </c>
       <c r="I63" t="b">
         <v>1</v>
       </c>
       <c r="J63" s="7" t="s">
-        <v>145</v>
+        <v>230</v>
       </c>
       <c r="K63">
-        <v>1000</v>
+        <v>30000</v>
       </c>
       <c r="L63">
-        <v>1000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
@@ -5752,7 +5708,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C64" t="s">
         <v>27</v>
@@ -5762,7 +5718,7 @@
         <v>2</v>
       </c>
       <c r="E64" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F64" t="s">
         <v>181</v>
@@ -5777,7 +5733,7 @@
         <v>1</v>
       </c>
       <c r="J64" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K64">
         <v>1000</v>
@@ -5791,7 +5747,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>88</v>
+        <v>36</v>
       </c>
       <c r="C65" t="s">
         <v>27</v>
@@ -5801,7 +5757,7 @@
         <v>2</v>
       </c>
       <c r="E65" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F65" t="s">
         <v>181</v>
@@ -5816,7 +5772,7 @@
         <v>1</v>
       </c>
       <c r="J65" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K65">
         <v>1000</v>
@@ -5830,7 +5786,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C66" t="s">
         <v>27</v>
@@ -5840,10 +5796,10 @@
         <v>2</v>
       </c>
       <c r="E66" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F66" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G66" t="s">
         <v>34</v>
@@ -5855,7 +5811,7 @@
         <v>1</v>
       </c>
       <c r="J66" s="7" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="K66">
         <v>1000</v>
@@ -5869,7 +5825,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C67" t="s">
         <v>27</v>
@@ -5879,22 +5835,22 @@
         <v>2</v>
       </c>
       <c r="E67" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F67" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G67" t="s">
-        <v>151</v>
+        <v>34</v>
       </c>
       <c r="H67" t="s">
-        <v>152</v>
+        <v>35</v>
       </c>
       <c r="I67" t="b">
         <v>1</v>
       </c>
       <c r="J67" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K67">
         <v>1000</v>
@@ -5908,7 +5864,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C68" t="s">
         <v>27</v>
@@ -5918,7 +5874,7 @@
         <v>2</v>
       </c>
       <c r="E68" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F68" t="s">
         <v>182</v>
@@ -5933,7 +5889,7 @@
         <v>1</v>
       </c>
       <c r="J68" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K68">
         <v>1000</v>
@@ -5947,7 +5903,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C69" t="s">
         <v>27</v>
@@ -5957,7 +5913,7 @@
         <v>2</v>
       </c>
       <c r="E69" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F69" t="s">
         <v>182</v>
@@ -5972,7 +5928,7 @@
         <v>1</v>
       </c>
       <c r="J69" s="7" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="K69">
         <v>1000</v>
@@ -5986,7 +5942,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C70" t="s">
         <v>27</v>
@@ -5996,10 +5952,10 @@
         <v>2</v>
       </c>
       <c r="E70" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F70" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G70" t="s">
         <v>34</v>
@@ -6011,7 +5967,7 @@
         <v>1</v>
       </c>
       <c r="J70" s="7" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="K70">
         <v>1000</v>
@@ -6025,7 +5981,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C71" t="s">
         <v>27</v>
@@ -6035,10 +5991,10 @@
         <v>2</v>
       </c>
       <c r="E71" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F71" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G71" t="s">
         <v>151</v>
@@ -6050,7 +6006,7 @@
         <v>1</v>
       </c>
       <c r="J71" s="7" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
       <c r="K71">
         <v>1000</v>
@@ -6064,7 +6020,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C72" t="s">
         <v>27</v>
@@ -6074,7 +6030,7 @@
         <v>2</v>
       </c>
       <c r="E72" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F72" t="s">
         <v>183</v>
@@ -6089,7 +6045,7 @@
         <v>1</v>
       </c>
       <c r="J72" s="7" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="K72">
         <v>1000</v>
@@ -6103,7 +6059,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C73" t="s">
         <v>27</v>
@@ -6113,7 +6069,7 @@
         <v>2</v>
       </c>
       <c r="E73" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F73" t="s">
         <v>183</v>
@@ -6128,7 +6084,7 @@
         <v>1</v>
       </c>
       <c r="J73" s="7" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="K73">
         <v>1000</v>
@@ -6142,7 +6098,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C74" t="s">
         <v>27</v>
@@ -6152,10 +6108,10 @@
         <v>2</v>
       </c>
       <c r="E74" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F74" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G74" t="s">
         <v>34</v>
@@ -6167,7 +6123,7 @@
         <v>1</v>
       </c>
       <c r="J74" s="7" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="K74">
         <v>1000</v>
@@ -6181,7 +6137,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C75" t="s">
         <v>27</v>
@@ -6191,10 +6147,10 @@
         <v>2</v>
       </c>
       <c r="E75" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F75" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G75" t="s">
         <v>151</v>
@@ -6206,7 +6162,7 @@
         <v>1</v>
       </c>
       <c r="J75" s="7" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="K75">
         <v>1000</v>
@@ -6220,7 +6176,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C76" t="s">
         <v>27</v>
@@ -6230,7 +6186,7 @@
         <v>2</v>
       </c>
       <c r="E76" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F76" t="s">
         <v>184</v>
@@ -6245,7 +6201,7 @@
         <v>1</v>
       </c>
       <c r="J76" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K76">
         <v>1000</v>
@@ -6259,7 +6215,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C77" t="s">
         <v>27</v>
@@ -6269,7 +6225,7 @@
         <v>2</v>
       </c>
       <c r="E77" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F77" t="s">
         <v>184</v>
@@ -6284,7 +6240,7 @@
         <v>1</v>
       </c>
       <c r="J77" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K77">
         <v>1000</v>
@@ -6298,7 +6254,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C78" t="s">
         <v>27</v>
@@ -6308,10 +6264,10 @@
         <v>2</v>
       </c>
       <c r="E78" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F78" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G78" t="s">
         <v>34</v>
@@ -6323,7 +6279,7 @@
         <v>1</v>
       </c>
       <c r="J78" s="7" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="K78">
         <v>1000</v>
@@ -6337,7 +6293,7 @@
         <v>77</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C79" t="s">
         <v>27</v>
@@ -6347,10 +6303,10 @@
         <v>2</v>
       </c>
       <c r="E79" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F79" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G79" t="s">
         <v>151</v>
@@ -6362,7 +6318,7 @@
         <v>1</v>
       </c>
       <c r="J79" s="7" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="K79">
         <v>1000</v>
@@ -6376,7 +6332,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C80" t="s">
         <v>27</v>
@@ -6386,7 +6342,7 @@
         <v>2</v>
       </c>
       <c r="E80" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F80" t="s">
         <v>185</v>
@@ -6401,7 +6357,7 @@
         <v>1</v>
       </c>
       <c r="J80" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K80">
         <v>1000</v>
@@ -6415,7 +6371,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C81" t="s">
         <v>27</v>
@@ -6425,7 +6381,7 @@
         <v>2</v>
       </c>
       <c r="E81" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F81" t="s">
         <v>185</v>
@@ -6440,7 +6396,7 @@
         <v>1</v>
       </c>
       <c r="J81" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K81">
         <v>1000</v>
@@ -6454,7 +6410,7 @@
         <v>80</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C82" t="s">
         <v>27</v>
@@ -6464,10 +6420,10 @@
         <v>2</v>
       </c>
       <c r="E82" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F82" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G82" t="s">
         <v>34</v>
@@ -6479,7 +6435,7 @@
         <v>1</v>
       </c>
       <c r="J82" s="7" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="K82">
         <v>1000</v>
@@ -6493,7 +6449,7 @@
         <v>81</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>221</v>
+        <v>104</v>
       </c>
       <c r="C83" t="s">
         <v>27</v>
@@ -6503,10 +6459,10 @@
         <v>2</v>
       </c>
       <c r="E83" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F83" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G83" t="s">
         <v>151</v>
@@ -6518,7 +6474,7 @@
         <v>1</v>
       </c>
       <c r="J83" s="7" t="s">
-        <v>223</v>
+        <v>172</v>
       </c>
       <c r="K83">
         <v>1000</v>
@@ -6532,7 +6488,7 @@
         <v>82</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C84" t="s">
         <v>27</v>
@@ -6542,7 +6498,7 @@
         <v>2</v>
       </c>
       <c r="E84" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F84" t="s">
         <v>186</v>
@@ -6557,7 +6513,7 @@
         <v>1</v>
       </c>
       <c r="J84" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K84">
         <v>1000</v>
@@ -6571,7 +6527,7 @@
         <v>83</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>107</v>
+        <v>219</v>
       </c>
       <c r="C85" t="s">
         <v>27</v>
@@ -6581,7 +6537,7 @@
         <v>2</v>
       </c>
       <c r="E85" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F85" t="s">
         <v>186</v>
@@ -6596,12 +6552,90 @@
         <v>1</v>
       </c>
       <c r="J85" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="K85">
+        <v>1000</v>
+      </c>
+      <c r="L85">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>84</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C86" t="s">
+        <v>27</v>
+      </c>
+      <c r="D86" s="5">
+        <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="E86" t="s">
+        <v>12</v>
+      </c>
+      <c r="F86" t="s">
+        <v>186</v>
+      </c>
+      <c r="G86" t="s">
+        <v>34</v>
+      </c>
+      <c r="H86" t="s">
+        <v>35</v>
+      </c>
+      <c r="I86" t="b">
+        <v>1</v>
+      </c>
+      <c r="J86" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="K86">
+        <v>1000</v>
+      </c>
+      <c r="L86">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>85</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C87" t="s">
+        <v>27</v>
+      </c>
+      <c r="D87" s="5">
+        <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="E87" t="s">
+        <v>13</v>
+      </c>
+      <c r="F87" t="s">
+        <v>186</v>
+      </c>
+      <c r="G87" t="s">
+        <v>151</v>
+      </c>
+      <c r="H87" t="s">
+        <v>152</v>
+      </c>
+      <c r="I87" t="b">
+        <v>1</v>
+      </c>
+      <c r="J87" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="K85">
-        <v>1000</v>
-      </c>
-      <c r="L85">
+      <c r="K87">
+        <v>1000</v>
+      </c>
+      <c r="L87">
         <v>1000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated config with new datasets
</commit_message>
<xml_diff>
--- a/model_config.xlsx
+++ b/model_config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asafsilman/Desktop/GENG5511/GalaxyEnvironmentAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCAB6A5-C79B-B344-A65B-C0425CC8BABD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6F490E-1763-2F4E-B4D2-A80B63E00036}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" activeTab="1" xr2:uid="{DA573336-42C9-534D-A3C9-C8C047CC3E2B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="254">
   <si>
     <t>modelName</t>
   </si>
@@ -776,6 +776,27 @@
   </si>
   <si>
     <t>63fd5dc85fb77e5cb9b4a54f02bfd265a697220cf24d6ee3c8b5adcb1e47107b</t>
+  </si>
+  <si>
+    <t>A.r.m14.dir.tar.gz</t>
+  </si>
+  <si>
+    <t>m11</t>
+  </si>
+  <si>
+    <t>A.t.m7v.dir.tar.gz</t>
+  </si>
+  <si>
+    <t>A.t.m7.dir.tar.gz</t>
+  </si>
+  <si>
+    <t>8b7c68e58d1a5d15eefe87f31d73f1227aab7b8ddcdd5f1f1913d13ba5d32161</t>
+  </si>
+  <si>
+    <t>ca1b56c74337b7a733bfdf6084a96efd27e148000121adf77188fa44bcd4c4d6</t>
+  </si>
+  <si>
+    <t>c9b727b12a4c5eedd272b44f7a8eaf2c8aca6de4a65503ca558f72905b59e73c</t>
   </si>
 </sst>
 </file>
@@ -984,8 +1005,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BBA15079-BA5C-4347-AB18-D63DE85A40E7}" name="Table1" displayName="Table1" ref="A1:L93" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:L93" xr:uid="{1608FF67-3914-5949-96DC-606C50EA2E4D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BBA15079-BA5C-4347-AB18-D63DE85A40E7}" name="Table1" displayName="Table1" ref="A1:L96" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:L96" xr:uid="{1608FF67-3914-5949-96DC-606C50EA2E4D}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{AE589D12-F9F2-7E46-B3F1-011FE87BB9E7}" name="dataId"/>
     <tableColumn id="2" xr3:uid="{86A820C4-44CA-F647-A338-3C42F8D54CAF}" name="dataFile" dataDxfId="5"/>
@@ -3272,10 +3293,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A15A60-C633-ED48-8690-686D42EE8C24}">
-  <dimension ref="A1:L93"/>
+  <dimension ref="A1:L96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K68" sqref="K68:L69"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72:XFD72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4271,20 +4292,20 @@
         <v>24</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>63</v>
+        <v>250</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D26" s="5">
         <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" t="s">
         <v>11</v>
       </c>
       <c r="F26" t="s">
-        <v>181</v>
+        <v>229</v>
       </c>
       <c r="G26" t="s">
         <v>34</v>
@@ -4296,13 +4317,13 @@
         <v>1</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>125</v>
+        <v>252</v>
       </c>
       <c r="K26">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="L26">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
@@ -4310,38 +4331,38 @@
         <v>25</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>64</v>
+        <v>249</v>
       </c>
       <c r="C27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D27" s="5">
         <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27" t="s">
         <v>14</v>
       </c>
       <c r="F27" t="s">
-        <v>181</v>
+        <v>229</v>
       </c>
       <c r="G27" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="H27" t="s">
-        <v>35</v>
+        <v>152</v>
       </c>
       <c r="I27" t="b">
         <v>1</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>126</v>
+        <v>253</v>
       </c>
       <c r="K27">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="L27">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
@@ -4349,7 +4370,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C28" t="s">
         <v>26</v>
@@ -4359,7 +4380,7 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F28" t="s">
         <v>181</v>
@@ -4374,7 +4395,7 @@
         <v>1</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K28">
         <v>1000</v>
@@ -4388,7 +4409,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C29" t="s">
         <v>26</v>
@@ -4398,7 +4419,7 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F29" t="s">
         <v>181</v>
@@ -4413,7 +4434,7 @@
         <v>1</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K29">
         <v>1000</v>
@@ -4427,7 +4448,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C30" t="s">
         <v>26</v>
@@ -4437,10 +4458,10 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F30" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G30" t="s">
         <v>34</v>
@@ -4452,7 +4473,7 @@
         <v>1</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K30">
         <v>1000</v>
@@ -4466,7 +4487,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C31" t="s">
         <v>26</v>
@@ -4476,10 +4497,10 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G31" t="s">
         <v>34</v>
@@ -4491,7 +4512,7 @@
         <v>1</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="K31">
         <v>1000</v>
@@ -4505,7 +4526,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C32" t="s">
         <v>26</v>
@@ -4515,7 +4536,7 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F32" t="s">
         <v>182</v>
@@ -4530,7 +4551,7 @@
         <v>1</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>160</v>
+        <v>129</v>
       </c>
       <c r="K32">
         <v>1000</v>
@@ -4544,7 +4565,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C33" t="s">
         <v>26</v>
@@ -4554,7 +4575,7 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F33" t="s">
         <v>182</v>
@@ -4569,7 +4590,7 @@
         <v>1</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="K33">
         <v>1000</v>
@@ -4583,7 +4604,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C34" t="s">
         <v>26</v>
@@ -4593,10 +4614,10 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F34" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G34" t="s">
         <v>34</v>
@@ -4608,7 +4629,7 @@
         <v>1</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>131</v>
+        <v>160</v>
       </c>
       <c r="K34">
         <v>1000</v>
@@ -4622,7 +4643,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C35" t="s">
         <v>26</v>
@@ -4632,10 +4653,10 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F35" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G35" t="s">
         <v>34</v>
@@ -4647,7 +4668,7 @@
         <v>1</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>132</v>
+        <v>161</v>
       </c>
       <c r="K35">
         <v>1000</v>
@@ -4661,7 +4682,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C36" t="s">
         <v>26</v>
@@ -4671,7 +4692,7 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F36" t="s">
         <v>183</v>
@@ -4686,7 +4707,7 @@
         <v>1</v>
       </c>
       <c r="J36" s="7" t="s">
-        <v>162</v>
+        <v>131</v>
       </c>
       <c r="K36">
         <v>1000</v>
@@ -4700,7 +4721,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C37" t="s">
         <v>26</v>
@@ -4710,7 +4731,7 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F37" t="s">
         <v>183</v>
@@ -4725,7 +4746,7 @@
         <v>1</v>
       </c>
       <c r="J37" s="7" t="s">
-        <v>163</v>
+        <v>132</v>
       </c>
       <c r="K37">
         <v>1000</v>
@@ -4739,7 +4760,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C38" t="s">
         <v>26</v>
@@ -4749,10 +4770,10 @@
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F38" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="G38" t="s">
         <v>34</v>
@@ -4764,13 +4785,13 @@
         <v>1</v>
       </c>
       <c r="J38" s="7" t="s">
-        <v>133</v>
+        <v>162</v>
       </c>
       <c r="K38">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="L38">
-        <v>500</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
@@ -4778,7 +4799,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C39" t="s">
         <v>26</v>
@@ -4788,28 +4809,28 @@
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F39" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="G39" t="s">
-        <v>151</v>
+        <v>34</v>
       </c>
       <c r="H39" t="s">
-        <v>152</v>
+        <v>35</v>
       </c>
       <c r="I39" t="b">
         <v>1</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>134</v>
+        <v>163</v>
       </c>
       <c r="K39">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="L39">
-        <v>500</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
@@ -4817,7 +4838,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C40" t="s">
         <v>26</v>
@@ -4827,7 +4848,7 @@
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F40" t="s">
         <v>199</v>
@@ -4842,7 +4863,7 @@
         <v>1</v>
       </c>
       <c r="J40" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K40">
         <v>500</v>
@@ -4856,7 +4877,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C41" t="s">
         <v>26</v>
@@ -4866,7 +4887,7 @@
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F41" t="s">
         <v>199</v>
@@ -4880,8 +4901,8 @@
       <c r="I41" t="b">
         <v>1</v>
       </c>
-      <c r="J41" s="6" t="s">
-        <v>136</v>
+      <c r="J41" s="7" t="s">
+        <v>134</v>
       </c>
       <c r="K41">
         <v>500</v>
@@ -4895,7 +4916,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C42" t="s">
         <v>26</v>
@@ -4905,10 +4926,10 @@
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F42" t="s">
-        <v>225</v>
+        <v>199</v>
       </c>
       <c r="G42" t="s">
         <v>34</v>
@@ -4919,8 +4940,8 @@
       <c r="I42" t="b">
         <v>1</v>
       </c>
-      <c r="J42" s="6" t="s">
-        <v>137</v>
+      <c r="J42" s="7" t="s">
+        <v>135</v>
       </c>
       <c r="K42">
         <v>500</v>
@@ -4934,7 +4955,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C43" t="s">
         <v>26</v>
@@ -4944,10 +4965,10 @@
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F43" t="s">
-        <v>225</v>
+        <v>199</v>
       </c>
       <c r="G43" t="s">
         <v>151</v>
@@ -4958,8 +4979,8 @@
       <c r="I43" t="b">
         <v>1</v>
       </c>
-      <c r="J43" s="7" t="s">
-        <v>138</v>
+      <c r="J43" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="K43">
         <v>500</v>
@@ -4973,7 +4994,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C44" t="s">
         <v>26</v>
@@ -4983,7 +5004,7 @@
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F44" t="s">
         <v>225</v>
@@ -4997,8 +5018,8 @@
       <c r="I44" t="b">
         <v>1</v>
       </c>
-      <c r="J44" s="7" t="s">
-        <v>139</v>
+      <c r="J44" s="6" t="s">
+        <v>137</v>
       </c>
       <c r="K44">
         <v>500</v>
@@ -5012,7 +5033,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C45" t="s">
         <v>26</v>
@@ -5022,7 +5043,7 @@
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F45" t="s">
         <v>225</v>
@@ -5037,7 +5058,7 @@
         <v>1</v>
       </c>
       <c r="J45" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K45">
         <v>500</v>
@@ -5051,7 +5072,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C46" t="s">
         <v>26</v>
@@ -5061,10 +5082,10 @@
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G46" t="s">
         <v>34</v>
@@ -5076,7 +5097,7 @@
         <v>1</v>
       </c>
       <c r="J46" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K46">
         <v>500</v>
@@ -5090,7 +5111,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>204</v>
+        <v>82</v>
       </c>
       <c r="C47" t="s">
         <v>26</v>
@@ -5100,10 +5121,10 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F47" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G47" t="s">
         <v>151</v>
@@ -5115,7 +5136,7 @@
         <v>1</v>
       </c>
       <c r="J47" s="7" t="s">
-        <v>208</v>
+        <v>140</v>
       </c>
       <c r="K47">
         <v>500</v>
@@ -5129,7 +5150,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C48" t="s">
         <v>26</v>
@@ -5139,7 +5160,7 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F48" t="s">
         <v>226</v>
@@ -5154,7 +5175,7 @@
         <v>1</v>
       </c>
       <c r="J48" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K48">
         <v>500</v>
@@ -5168,7 +5189,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>85</v>
+        <v>204</v>
       </c>
       <c r="C49" t="s">
         <v>26</v>
@@ -5178,7 +5199,7 @@
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F49" t="s">
         <v>226</v>
@@ -5193,7 +5214,7 @@
         <v>1</v>
       </c>
       <c r="J49" s="7" t="s">
-        <v>143</v>
+        <v>208</v>
       </c>
       <c r="K49">
         <v>500</v>
@@ -5207,7 +5228,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>190</v>
+        <v>84</v>
       </c>
       <c r="C50" t="s">
         <v>26</v>
@@ -5217,10 +5238,10 @@
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F50" t="s">
-        <v>184</v>
+        <v>226</v>
       </c>
       <c r="G50" t="s">
         <v>34</v>
@@ -5232,13 +5253,13 @@
         <v>1</v>
       </c>
       <c r="J50" s="7" t="s">
-        <v>203</v>
+        <v>142</v>
       </c>
       <c r="K50">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L50">
-        <v>1000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
@@ -5246,7 +5267,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>205</v>
+        <v>85</v>
       </c>
       <c r="C51" t="s">
         <v>26</v>
@@ -5256,10 +5277,10 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F51" t="s">
-        <v>184</v>
+        <v>226</v>
       </c>
       <c r="G51" t="s">
         <v>151</v>
@@ -5271,13 +5292,13 @@
         <v>1</v>
       </c>
       <c r="J51" s="7" t="s">
-        <v>209</v>
+        <v>143</v>
       </c>
       <c r="K51">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L51">
-        <v>1000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
@@ -5285,7 +5306,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C52" t="s">
         <v>26</v>
@@ -5295,7 +5316,7 @@
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F52" t="s">
         <v>184</v>
@@ -5310,7 +5331,7 @@
         <v>1</v>
       </c>
       <c r="J52" s="7" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="K52">
         <v>1000</v>
@@ -5324,7 +5345,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="C53" t="s">
         <v>26</v>
@@ -5334,7 +5355,7 @@
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F53" t="s">
         <v>184</v>
@@ -5349,7 +5370,7 @@
         <v>1</v>
       </c>
       <c r="J53" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K53">
         <v>1000</v>
@@ -5363,7 +5384,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C54" t="s">
         <v>26</v>
@@ -5373,10 +5394,10 @@
         <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F54" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G54" t="s">
         <v>34</v>
@@ -5388,7 +5409,7 @@
         <v>1</v>
       </c>
       <c r="J54" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="K54">
         <v>1000</v>
@@ -5402,7 +5423,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="C55" t="s">
         <v>26</v>
@@ -5412,10 +5433,10 @@
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F55" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G55" t="s">
         <v>151</v>
@@ -5427,7 +5448,7 @@
         <v>1</v>
       </c>
       <c r="J55" s="7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K55">
         <v>1000</v>
@@ -5441,7 +5462,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C56" t="s">
         <v>26</v>
@@ -5451,7 +5472,7 @@
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F56" t="s">
         <v>185</v>
@@ -5466,7 +5487,7 @@
         <v>1</v>
       </c>
       <c r="J56" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K56">
         <v>1000</v>
@@ -5480,7 +5501,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="C57" t="s">
         <v>26</v>
@@ -5490,7 +5511,7 @@
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F57" t="s">
         <v>185</v>
@@ -5505,7 +5526,7 @@
         <v>1</v>
       </c>
       <c r="J57" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K57">
         <v>1000</v>
@@ -5519,7 +5540,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C58" t="s">
         <v>26</v>
@@ -5529,10 +5550,10 @@
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F58" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G58" t="s">
         <v>34</v>
@@ -5544,7 +5565,7 @@
         <v>1</v>
       </c>
       <c r="J58" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="K58">
         <v>1000</v>
@@ -5558,7 +5579,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="C59" t="s">
         <v>26</v>
@@ -5568,10 +5589,10 @@
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F59" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G59" t="s">
         <v>151</v>
@@ -5583,7 +5604,7 @@
         <v>1</v>
       </c>
       <c r="J59" s="7" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="K59">
         <v>1000</v>
@@ -5597,7 +5618,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C60" t="s">
         <v>26</v>
@@ -5607,7 +5628,7 @@
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F60" t="s">
         <v>186</v>
@@ -5622,7 +5643,7 @@
         <v>1</v>
       </c>
       <c r="J60" s="7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="K60">
         <v>1000</v>
@@ -5636,7 +5657,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="C61" t="s">
         <v>26</v>
@@ -5646,7 +5667,7 @@
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F61" t="s">
         <v>186</v>
@@ -5661,7 +5682,7 @@
         <v>1</v>
       </c>
       <c r="J61" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="K61">
         <v>1000</v>
@@ -5675,7 +5696,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>227</v>
+        <v>197</v>
       </c>
       <c r="C62" t="s">
         <v>26</v>
@@ -5685,10 +5706,10 @@
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F62" t="s">
-        <v>229</v>
+        <v>186</v>
       </c>
       <c r="G62" t="s">
         <v>34</v>
@@ -5700,13 +5721,13 @@
         <v>1</v>
       </c>
       <c r="J62" s="7" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="K62">
-        <v>30000</v>
+        <v>1000</v>
       </c>
       <c r="L62">
-        <v>30000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
@@ -5714,7 +5735,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>228</v>
+        <v>198</v>
       </c>
       <c r="C63" t="s">
         <v>26</v>
@@ -5724,10 +5745,10 @@
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F63" t="s">
-        <v>229</v>
+        <v>186</v>
       </c>
       <c r="G63" t="s">
         <v>151</v>
@@ -5739,13 +5760,13 @@
         <v>1</v>
       </c>
       <c r="J63" s="7" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="K63">
-        <v>30000</v>
+        <v>1000</v>
       </c>
       <c r="L63">
-        <v>30000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
@@ -5753,7 +5774,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="C64" t="s">
         <v>26</v>
@@ -5766,7 +5787,7 @@
         <v>11</v>
       </c>
       <c r="F64" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="G64" t="s">
         <v>34</v>
@@ -5778,7 +5799,7 @@
         <v>1</v>
       </c>
       <c r="J64" s="7" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="K64">
         <v>30000</v>
@@ -5792,7 +5813,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C65" t="s">
         <v>26</v>
@@ -5805,7 +5826,7 @@
         <v>14</v>
       </c>
       <c r="F65" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="G65" t="s">
         <v>151</v>
@@ -5817,7 +5838,7 @@
         <v>1</v>
       </c>
       <c r="J65" s="7" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="K65">
         <v>30000</v>
@@ -5831,7 +5852,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C66" t="s">
         <v>26</v>
@@ -5844,7 +5865,7 @@
         <v>11</v>
       </c>
       <c r="F66" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G66" t="s">
         <v>34</v>
@@ -5856,7 +5877,7 @@
         <v>1</v>
       </c>
       <c r="J66" s="7" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K66">
         <v>30000</v>
@@ -5870,7 +5891,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C67" t="s">
         <v>26</v>
@@ -5883,7 +5904,7 @@
         <v>14</v>
       </c>
       <c r="F67" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G67" t="s">
         <v>151</v>
@@ -5895,7 +5916,7 @@
         <v>1</v>
       </c>
       <c r="J67" s="7" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K67">
         <v>30000</v>
@@ -5909,7 +5930,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="C68" t="s">
         <v>26</v>
@@ -5922,7 +5943,7 @@
         <v>11</v>
       </c>
       <c r="F68" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="G68" t="s">
         <v>34</v>
@@ -5934,7 +5955,7 @@
         <v>1</v>
       </c>
       <c r="J68" s="7" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="K68">
         <v>30000</v>
@@ -5948,7 +5969,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="C69" t="s">
         <v>26</v>
@@ -5961,7 +5982,7 @@
         <v>14</v>
       </c>
       <c r="F69" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="G69" t="s">
         <v>151</v>
@@ -5973,7 +5994,7 @@
         <v>1</v>
       </c>
       <c r="J69" s="7" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="K69">
         <v>30000</v>
@@ -5987,20 +6008,20 @@
         <v>68</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>86</v>
+        <v>243</v>
       </c>
       <c r="C70" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D70" s="5">
         <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E70" t="s">
         <v>11</v>
       </c>
       <c r="F70" t="s">
-        <v>181</v>
+        <v>242</v>
       </c>
       <c r="G70" t="s">
         <v>34</v>
@@ -6012,13 +6033,13 @@
         <v>1</v>
       </c>
       <c r="J70" s="7" t="s">
-        <v>144</v>
+        <v>245</v>
       </c>
       <c r="K70">
-        <v>1000</v>
+        <v>30000</v>
       </c>
       <c r="L70">
-        <v>1000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
@@ -6026,38 +6047,38 @@
         <v>69</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>36</v>
+        <v>244</v>
       </c>
       <c r="C71" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D71" s="5">
         <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E71" t="s">
         <v>14</v>
       </c>
       <c r="F71" t="s">
-        <v>181</v>
+        <v>242</v>
       </c>
       <c r="G71" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="H71" t="s">
-        <v>35</v>
+        <v>152</v>
       </c>
       <c r="I71" t="b">
         <v>1</v>
       </c>
       <c r="J71" s="7" t="s">
-        <v>145</v>
+        <v>246</v>
       </c>
       <c r="K71">
-        <v>1000</v>
+        <v>30000</v>
       </c>
       <c r="L71">
-        <v>1000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.2">
@@ -6065,20 +6086,20 @@
         <v>70</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>87</v>
+        <v>247</v>
       </c>
       <c r="C72" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D72" s="5">
         <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F72" t="s">
-        <v>181</v>
+        <v>248</v>
       </c>
       <c r="G72" t="s">
         <v>34</v>
@@ -6090,13 +6111,13 @@
         <v>1</v>
       </c>
       <c r="J72" s="7" t="s">
-        <v>146</v>
+        <v>251</v>
       </c>
       <c r="K72">
-        <v>1000</v>
+        <v>30000</v>
       </c>
       <c r="L72">
-        <v>1000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.2">
@@ -6104,7 +6125,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C73" t="s">
         <v>27</v>
@@ -6114,7 +6135,7 @@
         <v>2</v>
       </c>
       <c r="E73" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F73" t="s">
         <v>181</v>
@@ -6129,7 +6150,7 @@
         <v>1</v>
       </c>
       <c r="J73" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="K73">
         <v>1000</v>
@@ -6143,7 +6164,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>89</v>
+        <v>36</v>
       </c>
       <c r="C74" t="s">
         <v>27</v>
@@ -6153,10 +6174,10 @@
         <v>2</v>
       </c>
       <c r="E74" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F74" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G74" t="s">
         <v>34</v>
@@ -6168,7 +6189,7 @@
         <v>1</v>
       </c>
       <c r="J74" s="7" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="K74">
         <v>1000</v>
@@ -6182,7 +6203,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C75" t="s">
         <v>27</v>
@@ -6192,22 +6213,22 @@
         <v>2</v>
       </c>
       <c r="E75" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F75" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G75" t="s">
-        <v>151</v>
+        <v>34</v>
       </c>
       <c r="H75" t="s">
-        <v>152</v>
+        <v>35</v>
       </c>
       <c r="I75" t="b">
         <v>1</v>
       </c>
       <c r="J75" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K75">
         <v>1000</v>
@@ -6221,7 +6242,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C76" t="s">
         <v>27</v>
@@ -6231,10 +6252,10 @@
         <v>2</v>
       </c>
       <c r="E76" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F76" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G76" t="s">
         <v>34</v>
@@ -6246,7 +6267,7 @@
         <v>1</v>
       </c>
       <c r="J76" s="7" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="K76">
         <v>1000</v>
@@ -6260,7 +6281,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C77" t="s">
         <v>27</v>
@@ -6270,22 +6291,22 @@
         <v>2</v>
       </c>
       <c r="E77" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F77" t="s">
         <v>182</v>
       </c>
       <c r="G77" t="s">
-        <v>151</v>
+        <v>34</v>
       </c>
       <c r="H77" t="s">
-        <v>152</v>
+        <v>35</v>
       </c>
       <c r="I77" t="b">
         <v>1</v>
       </c>
       <c r="J77" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K77">
         <v>1000</v>
@@ -6299,7 +6320,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C78" t="s">
         <v>27</v>
@@ -6309,22 +6330,22 @@
         <v>2</v>
       </c>
       <c r="E78" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F78" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G78" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="H78" t="s">
-        <v>35</v>
+        <v>152</v>
       </c>
       <c r="I78" t="b">
         <v>1</v>
       </c>
       <c r="J78" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K78">
         <v>1000</v>
@@ -6338,7 +6359,7 @@
         <v>77</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C79" t="s">
         <v>27</v>
@@ -6348,22 +6369,22 @@
         <v>2</v>
       </c>
       <c r="E79" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F79" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G79" t="s">
-        <v>151</v>
+        <v>34</v>
       </c>
       <c r="H79" t="s">
-        <v>152</v>
+        <v>35</v>
       </c>
       <c r="I79" t="b">
         <v>1</v>
       </c>
       <c r="J79" s="7" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="K79">
         <v>1000</v>
@@ -6377,7 +6398,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C80" t="s">
         <v>27</v>
@@ -6387,22 +6408,22 @@
         <v>2</v>
       </c>
       <c r="E80" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F80" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G80" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="H80" t="s">
-        <v>35</v>
+        <v>152</v>
       </c>
       <c r="I80" t="b">
         <v>1</v>
       </c>
       <c r="J80" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K80">
         <v>1000</v>
@@ -6416,7 +6437,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C81" t="s">
         <v>27</v>
@@ -6426,22 +6447,22 @@
         <v>2</v>
       </c>
       <c r="E81" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F81" t="s">
         <v>183</v>
       </c>
       <c r="G81" t="s">
-        <v>151</v>
+        <v>34</v>
       </c>
       <c r="H81" t="s">
-        <v>152</v>
+        <v>35</v>
       </c>
       <c r="I81" t="b">
         <v>1</v>
       </c>
       <c r="J81" s="7" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="K81">
         <v>1000</v>
@@ -6455,7 +6476,7 @@
         <v>80</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C82" t="s">
         <v>27</v>
@@ -6465,22 +6486,22 @@
         <v>2</v>
       </c>
       <c r="E82" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F82" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G82" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="H82" t="s">
-        <v>35</v>
+        <v>152</v>
       </c>
       <c r="I82" t="b">
         <v>1</v>
       </c>
       <c r="J82" s="7" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="K82">
         <v>1000</v>
@@ -6494,7 +6515,7 @@
         <v>81</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C83" t="s">
         <v>27</v>
@@ -6504,22 +6525,22 @@
         <v>2</v>
       </c>
       <c r="E83" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F83" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G83" t="s">
-        <v>151</v>
+        <v>34</v>
       </c>
       <c r="H83" t="s">
-        <v>152</v>
+        <v>35</v>
       </c>
       <c r="I83" t="b">
         <v>1</v>
       </c>
       <c r="J83" s="7" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="K83">
         <v>1000</v>
@@ -6533,7 +6554,7 @@
         <v>82</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C84" t="s">
         <v>27</v>
@@ -6543,22 +6564,22 @@
         <v>2</v>
       </c>
       <c r="E84" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F84" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G84" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="H84" t="s">
-        <v>35</v>
+        <v>152</v>
       </c>
       <c r="I84" t="b">
         <v>1</v>
       </c>
       <c r="J84" s="7" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="K84">
         <v>1000</v>
@@ -6572,7 +6593,7 @@
         <v>83</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C85" t="s">
         <v>27</v>
@@ -6582,22 +6603,22 @@
         <v>2</v>
       </c>
       <c r="E85" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F85" t="s">
         <v>184</v>
       </c>
       <c r="G85" t="s">
-        <v>151</v>
+        <v>34</v>
       </c>
       <c r="H85" t="s">
-        <v>152</v>
+        <v>35</v>
       </c>
       <c r="I85" t="b">
         <v>1</v>
       </c>
       <c r="J85" s="7" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="K85">
         <v>1000</v>
@@ -6611,7 +6632,7 @@
         <v>84</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C86" t="s">
         <v>27</v>
@@ -6621,22 +6642,22 @@
         <v>2</v>
       </c>
       <c r="E86" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F86" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G86" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="H86" t="s">
-        <v>35</v>
+        <v>152</v>
       </c>
       <c r="I86" t="b">
         <v>1</v>
       </c>
       <c r="J86" s="7" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="K86">
         <v>1000</v>
@@ -6650,7 +6671,7 @@
         <v>85</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C87" t="s">
         <v>27</v>
@@ -6660,22 +6681,22 @@
         <v>2</v>
       </c>
       <c r="E87" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F87" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G87" t="s">
-        <v>151</v>
+        <v>34</v>
       </c>
       <c r="H87" t="s">
-        <v>152</v>
+        <v>35</v>
       </c>
       <c r="I87" t="b">
         <v>1</v>
       </c>
       <c r="J87" s="7" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="K87">
         <v>1000</v>
@@ -6689,7 +6710,7 @@
         <v>86</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C88" t="s">
         <v>27</v>
@@ -6699,22 +6720,22 @@
         <v>2</v>
       </c>
       <c r="E88" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F88" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G88" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="H88" t="s">
-        <v>35</v>
+        <v>152</v>
       </c>
       <c r="I88" t="b">
         <v>1</v>
       </c>
       <c r="J88" s="7" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="K88">
         <v>1000</v>
@@ -6728,7 +6749,7 @@
         <v>87</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C89" t="s">
         <v>27</v>
@@ -6738,22 +6759,22 @@
         <v>2</v>
       </c>
       <c r="E89" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F89" t="s">
         <v>185</v>
       </c>
       <c r="G89" t="s">
-        <v>151</v>
+        <v>34</v>
       </c>
       <c r="H89" t="s">
-        <v>152</v>
+        <v>35</v>
       </c>
       <c r="I89" t="b">
         <v>1</v>
       </c>
       <c r="J89" s="7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="K89">
         <v>1000</v>
@@ -6767,7 +6788,7 @@
         <v>88</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C90" t="s">
         <v>27</v>
@@ -6777,22 +6798,22 @@
         <v>2</v>
       </c>
       <c r="E90" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F90" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G90" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="H90" t="s">
-        <v>35</v>
+        <v>152</v>
       </c>
       <c r="I90" t="b">
         <v>1</v>
       </c>
       <c r="J90" s="7" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="K90">
         <v>1000</v>
@@ -6806,7 +6827,7 @@
         <v>89</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>219</v>
+        <v>103</v>
       </c>
       <c r="C91" t="s">
         <v>27</v>
@@ -6816,22 +6837,22 @@
         <v>2</v>
       </c>
       <c r="E91" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F91" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G91" t="s">
-        <v>151</v>
+        <v>34</v>
       </c>
       <c r="H91" t="s">
-        <v>152</v>
+        <v>35</v>
       </c>
       <c r="I91" t="b">
         <v>1</v>
       </c>
       <c r="J91" s="7" t="s">
-        <v>221</v>
+        <v>171</v>
       </c>
       <c r="K91">
         <v>1000</v>
@@ -6845,7 +6866,7 @@
         <v>90</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C92" t="s">
         <v>27</v>
@@ -6855,22 +6876,22 @@
         <v>2</v>
       </c>
       <c r="E92" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F92" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G92" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="H92" t="s">
-        <v>35</v>
+        <v>152</v>
       </c>
       <c r="I92" t="b">
         <v>1</v>
       </c>
       <c r="J92" s="7" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="K92">
         <v>1000</v>
@@ -6884,7 +6905,7 @@
         <v>91</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C93" t="s">
         <v>27</v>
@@ -6894,27 +6915,144 @@
         <v>2</v>
       </c>
       <c r="E93" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F93" t="s">
         <v>186</v>
       </c>
       <c r="G93" t="s">
+        <v>34</v>
+      </c>
+      <c r="H93" t="s">
+        <v>35</v>
+      </c>
+      <c r="I93" t="b">
+        <v>1</v>
+      </c>
+      <c r="J93" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="K93">
+        <v>1000</v>
+      </c>
+      <c r="L93">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>92</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="C94" t="s">
+        <v>27</v>
+      </c>
+      <c r="D94" s="5">
+        <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="E94" t="s">
+        <v>14</v>
+      </c>
+      <c r="F94" t="s">
+        <v>186</v>
+      </c>
+      <c r="G94" t="s">
         <v>151</v>
       </c>
-      <c r="H93" t="s">
+      <c r="H94" t="s">
         <v>152</v>
       </c>
-      <c r="I93" t="b">
-        <v>1</v>
-      </c>
-      <c r="J93" s="7" t="s">
+      <c r="I94" t="b">
+        <v>1</v>
+      </c>
+      <c r="J94" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="K94">
+        <v>1000</v>
+      </c>
+      <c r="L94">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>93</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C95" t="s">
+        <v>27</v>
+      </c>
+      <c r="D95" s="5">
+        <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="E95" t="s">
+        <v>12</v>
+      </c>
+      <c r="F95" t="s">
+        <v>186</v>
+      </c>
+      <c r="G95" t="s">
+        <v>34</v>
+      </c>
+      <c r="H95" t="s">
+        <v>35</v>
+      </c>
+      <c r="I95" t="b">
+        <v>1</v>
+      </c>
+      <c r="J95" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="K95">
+        <v>1000</v>
+      </c>
+      <c r="L95">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>94</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C96" t="s">
+        <v>27</v>
+      </c>
+      <c r="D96" s="5">
+        <f>VLOOKUP(Table1[[#This Row],[dataLabel]],Table2[#All],2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="E96" t="s">
+        <v>13</v>
+      </c>
+      <c r="F96" t="s">
+        <v>186</v>
+      </c>
+      <c r="G96" t="s">
+        <v>151</v>
+      </c>
+      <c r="H96" t="s">
+        <v>152</v>
+      </c>
+      <c r="I96" t="b">
+        <v>1</v>
+      </c>
+      <c r="J96" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="K93">
-        <v>1000</v>
-      </c>
-      <c r="L93">
+      <c r="K96">
+        <v>1000</v>
+      </c>
+      <c r="L96">
         <v>1000</v>
       </c>
     </row>

</xml_diff>